<commit_message>
Fix issue #9: all checks doing in lower case
</commit_message>
<xml_diff>
--- a/frontui/app_data/valar_report_tmpl.xlsx
+++ b/frontui/app_data/valar_report_tmpl.xlsx
@@ -94,6 +94,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Report!$A$1:$EE$78</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Report!$A$1:$EE$78</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">Report!$A$1:$EE$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">Report!$A$1:$EE$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">Report!$A$1:$EE$78</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -105,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="241">
   <si>
     <t xml:space="preserve">Тайный покупатель</t>
   </si>
@@ -993,48 +995,6 @@
   <si>
     <t xml:space="preserve">Атмосфера</t>
   </si>
-  <si>
-    <t xml:space="preserve">средний</t>
-  </si>
-  <si>
-    <t xml:space="preserve">нормальный</t>
-  </si>
-  <si>
-    <t xml:space="preserve">полный </t>
-  </si>
-  <si>
-    <t xml:space="preserve">пластиковый стаканчик </t>
-  </si>
-  <si>
-    <t xml:space="preserve">керамическая чашка</t>
-  </si>
-  <si>
-    <t xml:space="preserve">бумажный стаканчик </t>
-  </si>
-  <si>
-    <t xml:space="preserve">густая</t>
-  </si>
-  <si>
-    <t xml:space="preserve">американо</t>
-  </si>
-  <si>
-    <t xml:space="preserve">стойкая</t>
-  </si>
-  <si>
-    <t xml:space="preserve">крепкая</t>
-  </si>
-  <si>
-    <t xml:space="preserve">очень вкусный</t>
-  </si>
-  <si>
-    <t xml:space="preserve">не доброжелательная</t>
-  </si>
-  <si>
-    <t xml:space="preserve">гостеприимная</t>
-  </si>
-  <si>
-    <t xml:space="preserve">нейтральная</t>
-  </si>
 </sst>
 </file>
 
@@ -1049,7 +1009,7 @@
     <numFmt numFmtId="169" formatCode="H:MM;@"/>
     <numFmt numFmtId="170" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1237,27 +1197,6 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1285,7 +1224,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1305,27 +1244,6 @@
       <right/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top/>
-      <bottom style="medium"/>
       <diagonal/>
     </border>
   </borders>
@@ -1354,7 +1272,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="68">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1600,19 +1518,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="170" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="170" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1623,10 +1533,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1635,44 +1541,8 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -16357,95 +16227,95 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:KE104"/>
+  <dimension ref="A1:KE81"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="DL1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="DL1" activeCellId="0" sqref="DL1"/>
-      <selection pane="bottomLeft" activeCell="EB11" activeCellId="0" sqref="EB11"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="5" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="N77" activeCellId="0" sqref="N77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="3" style="2" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="3" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="3" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="3" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="18" min="15" style="3" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="20" min="19" style="3" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="3" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="2" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="3" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="3" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="3" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="18" min="15" style="3" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="20" min="19" style="3" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="3" width="16.7397959183673"/>
     <col collapsed="false" hidden="false" max="23" min="22" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="29" min="24" style="2" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="2" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="2" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="3" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="3" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="3" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="3" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="3" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="3" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="3" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="40" min="39" style="3" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="3" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="43" min="42" style="3" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="3" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="3" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="29" min="24" style="2" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="2" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="2" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="3" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="3" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="3" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="3" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="3" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="3" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="3" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="40" min="39" style="3" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="3" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="43" min="42" style="3" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="3" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="3" width="18.0867346938776"/>
     <col collapsed="false" hidden="false" max="46" min="46" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="52" min="47" style="2" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="2" width="5.82142857142857"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="2" width="24.8214285714286"/>
-    <col collapsed="false" hidden="false" max="56" min="55" style="3" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="3" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="58" min="58" style="3" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="59" min="59" style="3" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="60" min="60" style="3" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="61" min="61" style="3" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="63" min="62" style="3" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="65" min="64" style="3" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="66" min="66" style="3" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="67" min="67" style="3" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="68" min="68" style="3" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="52" min="47" style="2" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="2" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="2" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="56" min="55" style="3" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="3" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="58" min="58" style="3" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="59" min="59" style="3" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="60" min="60" style="3" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="61" min="61" style="3" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="63" min="62" style="3" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="65" min="64" style="3" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="66" min="66" style="3" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="67" min="67" style="3" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="68" min="68" style="3" width="16.7397959183673"/>
     <col collapsed="false" hidden="false" max="69" min="69" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="75" min="70" style="2" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="76" min="76" style="2" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="77" min="77" style="2" width="27.0816326530612"/>
-    <col collapsed="false" hidden="false" max="79" min="78" style="3" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="80" min="80" style="3" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="81" min="81" style="3" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="82" min="82" style="2" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="83" min="83" style="3" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="84" min="84" style="4" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="85" min="85" style="3" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="86" min="86" style="3" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="87" min="87" style="3" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="88" min="88" style="3" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="89" min="89" style="3" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="90" min="90" style="3" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="91" min="91" style="3" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="75" min="70" style="2" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="76" min="76" style="2" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="77" min="77" style="2" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="79" min="78" style="3" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="80" min="80" style="3" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="81" min="81" style="3" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="82" min="82" style="2" width="20.25"/>
+    <col collapsed="false" hidden="false" max="83" min="83" style="3" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="84" min="84" style="4" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="85" min="85" style="3" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="86" min="86" style="3" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="87" min="87" style="3" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="88" min="88" style="3" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="89" min="89" style="3" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="90" min="90" style="3" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="91" min="91" style="3" width="16.7397959183673"/>
     <col collapsed="false" hidden="false" max="92" min="92" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="98" min="93" style="2" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="99" min="99" style="2" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="100" min="100" style="2" width="25.7857142857143"/>
-    <col collapsed="false" hidden="false" max="101" min="101" style="3" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="105" min="102" style="3" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="107" min="106" style="3" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="110" min="108" style="3" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="114" min="111" style="3" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="98" min="93" style="2" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="99" min="99" style="2" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="100" min="100" style="2" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="101" min="101" style="3" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="105" min="102" style="3" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="107" min="106" style="3" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="110" min="108" style="3" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="114" min="111" style="3" width="16.7397959183673"/>
     <col collapsed="false" hidden="false" max="115" min="115" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="121" min="116" style="2" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="122" min="122" style="2" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="123" min="123" style="2" width="28.2040816326531"/>
-    <col collapsed="false" hidden="false" max="124" min="124" style="3" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="126" min="125" style="3" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="128" min="127" style="3" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="133" min="129" style="3" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="134" min="134" style="4" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="135" min="135" style="3" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="136" min="136" style="2" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="137" style="2" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="121" min="116" style="2" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="122" min="122" style="2" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="123" min="123" style="2" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="124" min="124" style="3" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="126" min="125" style="3" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="128" min="127" style="3" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="133" min="129" style="3" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="134" min="134" style="4" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="135" min="135" style="3" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="136" min="136" style="2" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="137" style="2" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -29350,7 +29220,9 @@
       <c r="EE69" s="47"/>
     </row>
     <row r="70" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="61"/>
+      <c r="A70" s="61" t="s">
+        <v>232</v>
+      </c>
       <c r="B70" s="61"/>
       <c r="C70" s="61"/>
       <c r="D70" s="61"/>
@@ -29359,147 +29231,147 @@
       <c r="G70" s="61"/>
       <c r="H70" s="61"/>
       <c r="I70" s="61"/>
-      <c r="J70" s="62" t="s">
+      <c r="J70" s="61"/>
+      <c r="K70" s="62"/>
+      <c r="L70" s="62"/>
+      <c r="M70" s="62"/>
+      <c r="N70" s="62"/>
+      <c r="O70" s="62"/>
+      <c r="P70" s="62"/>
+      <c r="Q70" s="62"/>
+      <c r="R70" s="62"/>
+      <c r="S70" s="62"/>
+      <c r="T70" s="62"/>
+      <c r="U70" s="62"/>
+      <c r="V70" s="61" t="s">
         <v>232</v>
       </c>
-      <c r="K70" s="63"/>
-      <c r="L70" s="63"/>
-      <c r="M70" s="63"/>
-      <c r="N70" s="63"/>
-      <c r="O70" s="63"/>
-      <c r="P70" s="63"/>
-      <c r="Q70" s="63"/>
-      <c r="R70" s="63"/>
-      <c r="S70" s="63"/>
-      <c r="T70" s="63"/>
-      <c r="U70" s="63"/>
-      <c r="V70" s="61"/>
       <c r="W70" s="61"/>
-      <c r="X70" s="64"/>
-      <c r="Y70" s="64"/>
-      <c r="Z70" s="64"/>
-      <c r="AA70" s="64"/>
-      <c r="AB70" s="64"/>
-      <c r="AC70" s="64"/>
-      <c r="AD70" s="64"/>
-      <c r="AE70" s="62" t="s">
+      <c r="X70" s="61"/>
+      <c r="Y70" s="61"/>
+      <c r="Z70" s="61"/>
+      <c r="AA70" s="61"/>
+      <c r="AB70" s="61"/>
+      <c r="AC70" s="61"/>
+      <c r="AD70" s="61"/>
+      <c r="AE70" s="61"/>
+      <c r="AF70" s="63"/>
+      <c r="AG70" s="63"/>
+      <c r="AH70" s="63"/>
+      <c r="AI70" s="63"/>
+      <c r="AJ70" s="63"/>
+      <c r="AK70" s="63"/>
+      <c r="AL70" s="63"/>
+      <c r="AM70" s="63"/>
+      <c r="AN70" s="63"/>
+      <c r="AO70" s="63"/>
+      <c r="AP70" s="63"/>
+      <c r="AQ70" s="63"/>
+      <c r="AR70" s="63"/>
+      <c r="AS70" s="63"/>
+      <c r="AT70" s="61" t="s">
         <v>232</v>
       </c>
-      <c r="AF70" s="65"/>
-      <c r="AG70" s="65"/>
-      <c r="AH70" s="65"/>
-      <c r="AI70" s="65"/>
-      <c r="AJ70" s="65"/>
-      <c r="AK70" s="65"/>
-      <c r="AL70" s="65"/>
-      <c r="AM70" s="65"/>
-      <c r="AN70" s="65"/>
-      <c r="AO70" s="65"/>
-      <c r="AP70" s="65"/>
-      <c r="AQ70" s="65"/>
-      <c r="AR70" s="65"/>
-      <c r="AS70" s="65"/>
-      <c r="AT70" s="61"/>
-      <c r="AU70" s="64"/>
-      <c r="AV70" s="64"/>
-      <c r="AW70" s="64"/>
-      <c r="AX70" s="64"/>
-      <c r="AY70" s="64"/>
-      <c r="AZ70" s="64"/>
-      <c r="BA70" s="64"/>
-      <c r="BB70" s="62" t="s">
+      <c r="AU70" s="61"/>
+      <c r="AV70" s="61"/>
+      <c r="AW70" s="61"/>
+      <c r="AX70" s="61"/>
+      <c r="AY70" s="61"/>
+      <c r="AZ70" s="61"/>
+      <c r="BA70" s="61"/>
+      <c r="BB70" s="61"/>
+      <c r="BC70" s="64"/>
+      <c r="BD70" s="64"/>
+      <c r="BE70" s="64"/>
+      <c r="BF70" s="64"/>
+      <c r="BG70" s="64"/>
+      <c r="BH70" s="64"/>
+      <c r="BI70" s="64"/>
+      <c r="BJ70" s="64"/>
+      <c r="BK70" s="64"/>
+      <c r="BL70" s="64"/>
+      <c r="BM70" s="64"/>
+      <c r="BN70" s="64"/>
+      <c r="BO70" s="64"/>
+      <c r="BP70" s="64"/>
+      <c r="BQ70" s="61" t="s">
         <v>232</v>
       </c>
-      <c r="BC70" s="66"/>
-      <c r="BD70" s="66"/>
-      <c r="BE70" s="66"/>
-      <c r="BF70" s="66"/>
-      <c r="BG70" s="66"/>
-      <c r="BH70" s="66"/>
-      <c r="BI70" s="66"/>
-      <c r="BJ70" s="66"/>
-      <c r="BK70" s="66"/>
-      <c r="BL70" s="66"/>
-      <c r="BM70" s="66"/>
-      <c r="BN70" s="66"/>
-      <c r="BO70" s="66"/>
-      <c r="BP70" s="66"/>
-      <c r="BQ70" s="61"/>
-      <c r="BR70" s="64"/>
-      <c r="BS70" s="64"/>
-      <c r="BT70" s="64"/>
-      <c r="BU70" s="64"/>
-      <c r="BV70" s="64"/>
-      <c r="BW70" s="64"/>
-      <c r="BX70" s="64"/>
-      <c r="BY70" s="62" t="s">
+      <c r="BR70" s="61"/>
+      <c r="BS70" s="61"/>
+      <c r="BT70" s="61"/>
+      <c r="BU70" s="61"/>
+      <c r="BV70" s="61"/>
+      <c r="BW70" s="61"/>
+      <c r="BX70" s="61"/>
+      <c r="BY70" s="61"/>
+      <c r="BZ70" s="64"/>
+      <c r="CA70" s="64"/>
+      <c r="CB70" s="64"/>
+      <c r="CC70" s="64"/>
+      <c r="CD70" s="64"/>
+      <c r="CE70" s="64"/>
+      <c r="CF70" s="64"/>
+      <c r="CG70" s="64"/>
+      <c r="CH70" s="64"/>
+      <c r="CI70" s="64"/>
+      <c r="CJ70" s="64"/>
+      <c r="CK70" s="64"/>
+      <c r="CL70" s="64"/>
+      <c r="CM70" s="64"/>
+      <c r="CN70" s="61" t="s">
         <v>232</v>
       </c>
-      <c r="BZ70" s="66"/>
-      <c r="CA70" s="66"/>
-      <c r="CB70" s="66"/>
-      <c r="CC70" s="66"/>
-      <c r="CD70" s="66"/>
-      <c r="CE70" s="66"/>
-      <c r="CF70" s="66"/>
-      <c r="CG70" s="66"/>
-      <c r="CH70" s="66"/>
-      <c r="CI70" s="66"/>
-      <c r="CJ70" s="66"/>
-      <c r="CK70" s="66"/>
-      <c r="CL70" s="66"/>
-      <c r="CM70" s="66"/>
-      <c r="CN70" s="61"/>
-      <c r="CO70" s="64"/>
-      <c r="CP70" s="64"/>
-      <c r="CQ70" s="64"/>
-      <c r="CR70" s="64"/>
-      <c r="CS70" s="64"/>
-      <c r="CT70" s="64"/>
-      <c r="CU70" s="64"/>
-      <c r="CV70" s="62" t="s">
+      <c r="CO70" s="61"/>
+      <c r="CP70" s="61"/>
+      <c r="CQ70" s="61"/>
+      <c r="CR70" s="61"/>
+      <c r="CS70" s="61"/>
+      <c r="CT70" s="61"/>
+      <c r="CU70" s="61"/>
+      <c r="CV70" s="61"/>
+      <c r="CW70" s="64"/>
+      <c r="CX70" s="64"/>
+      <c r="CY70" s="64"/>
+      <c r="CZ70" s="64"/>
+      <c r="DA70" s="64"/>
+      <c r="DB70" s="64"/>
+      <c r="DC70" s="64"/>
+      <c r="DD70" s="64"/>
+      <c r="DE70" s="64"/>
+      <c r="DF70" s="64"/>
+      <c r="DG70" s="64"/>
+      <c r="DH70" s="64"/>
+      <c r="DI70" s="64"/>
+      <c r="DJ70" s="64"/>
+      <c r="DK70" s="61" t="s">
         <v>232</v>
       </c>
-      <c r="CW70" s="66"/>
-      <c r="CX70" s="66"/>
-      <c r="CY70" s="66"/>
-      <c r="CZ70" s="66"/>
-      <c r="DA70" s="66"/>
-      <c r="DB70" s="66"/>
-      <c r="DC70" s="66"/>
-      <c r="DD70" s="66"/>
-      <c r="DE70" s="66"/>
-      <c r="DF70" s="66"/>
-      <c r="DG70" s="66"/>
-      <c r="DH70" s="66"/>
-      <c r="DI70" s="66"/>
-      <c r="DJ70" s="66"/>
-      <c r="DK70" s="61"/>
-      <c r="DL70" s="64"/>
-      <c r="DM70" s="64"/>
-      <c r="DN70" s="64"/>
-      <c r="DO70" s="64"/>
-      <c r="DP70" s="64"/>
-      <c r="DQ70" s="64"/>
-      <c r="DR70" s="64"/>
-      <c r="DS70" s="62" t="s">
-        <v>232</v>
-      </c>
-      <c r="DT70" s="66"/>
-      <c r="DU70" s="66"/>
-      <c r="DV70" s="66"/>
-      <c r="DW70" s="66"/>
-      <c r="DX70" s="66"/>
-      <c r="DY70" s="66"/>
-      <c r="DZ70" s="66"/>
-      <c r="EA70" s="66"/>
-      <c r="EB70" s="66"/>
-      <c r="EC70" s="66"/>
-      <c r="ED70" s="66"/>
-      <c r="EE70" s="66"/>
+      <c r="DL70" s="61"/>
+      <c r="DM70" s="61"/>
+      <c r="DN70" s="61"/>
+      <c r="DO70" s="61"/>
+      <c r="DP70" s="61"/>
+      <c r="DQ70" s="61"/>
+      <c r="DR70" s="61"/>
+      <c r="DS70" s="61"/>
+      <c r="DT70" s="64"/>
+      <c r="DU70" s="64"/>
+      <c r="DV70" s="64"/>
+      <c r="DW70" s="64"/>
+      <c r="DX70" s="64"/>
+      <c r="DY70" s="64"/>
+      <c r="DZ70" s="64"/>
+      <c r="EA70" s="64"/>
+      <c r="EB70" s="64"/>
+      <c r="EC70" s="64"/>
+      <c r="ED70" s="64"/>
+      <c r="EE70" s="64"/>
     </row>
     <row r="71" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="61"/>
+      <c r="A71" s="61" t="s">
+        <v>233</v>
+      </c>
       <c r="B71" s="61"/>
       <c r="C71" s="61"/>
       <c r="D71" s="61"/>
@@ -29508,9 +29380,7 @@
       <c r="G71" s="61"/>
       <c r="H71" s="61"/>
       <c r="I71" s="61"/>
-      <c r="J71" s="62" t="s">
-        <v>233</v>
-      </c>
+      <c r="J71" s="61"/>
       <c r="K71" s="39"/>
       <c r="L71" s="39"/>
       <c r="M71" s="39"/>
@@ -29522,18 +29392,18 @@
       <c r="S71" s="51"/>
       <c r="T71" s="51"/>
       <c r="U71" s="39"/>
-      <c r="V71" s="61"/>
+      <c r="V71" s="61" t="s">
+        <v>233</v>
+      </c>
       <c r="W71" s="61"/>
-      <c r="X71" s="64"/>
-      <c r="Y71" s="64"/>
-      <c r="Z71" s="64"/>
-      <c r="AA71" s="64"/>
-      <c r="AB71" s="64"/>
-      <c r="AC71" s="64"/>
-      <c r="AD71" s="64"/>
-      <c r="AE71" s="62" t="s">
-        <v>233</v>
-      </c>
+      <c r="X71" s="61"/>
+      <c r="Y71" s="61"/>
+      <c r="Z71" s="61"/>
+      <c r="AA71" s="61"/>
+      <c r="AB71" s="61"/>
+      <c r="AC71" s="61"/>
+      <c r="AD71" s="61"/>
+      <c r="AE71" s="61"/>
       <c r="AF71" s="47"/>
       <c r="AG71" s="47"/>
       <c r="AH71" s="49"/>
@@ -29548,17 +29418,17 @@
       <c r="AQ71" s="49"/>
       <c r="AR71" s="49"/>
       <c r="AS71" s="49"/>
-      <c r="AT71" s="61"/>
-      <c r="AU71" s="64"/>
-      <c r="AV71" s="64"/>
-      <c r="AW71" s="64"/>
-      <c r="AX71" s="64"/>
-      <c r="AY71" s="64"/>
-      <c r="AZ71" s="64"/>
-      <c r="BA71" s="64"/>
-      <c r="BB71" s="62" t="s">
+      <c r="AT71" s="61" t="s">
         <v>233</v>
       </c>
+      <c r="AU71" s="61"/>
+      <c r="AV71" s="61"/>
+      <c r="AW71" s="61"/>
+      <c r="AX71" s="61"/>
+      <c r="AY71" s="61"/>
+      <c r="AZ71" s="61"/>
+      <c r="BA71" s="61"/>
+      <c r="BB71" s="61"/>
       <c r="BC71" s="49"/>
       <c r="BD71" s="47"/>
       <c r="BE71" s="49"/>
@@ -29573,17 +29443,17 @@
       <c r="BN71" s="49"/>
       <c r="BO71" s="49"/>
       <c r="BP71" s="49"/>
-      <c r="BQ71" s="61"/>
-      <c r="BR71" s="64"/>
-      <c r="BS71" s="64"/>
-      <c r="BT71" s="64"/>
-      <c r="BU71" s="64"/>
-      <c r="BV71" s="64"/>
-      <c r="BW71" s="64"/>
-      <c r="BX71" s="64"/>
-      <c r="BY71" s="62" t="s">
+      <c r="BQ71" s="61" t="s">
         <v>233</v>
       </c>
+      <c r="BR71" s="61"/>
+      <c r="BS71" s="61"/>
+      <c r="BT71" s="61"/>
+      <c r="BU71" s="61"/>
+      <c r="BV71" s="61"/>
+      <c r="BW71" s="61"/>
+      <c r="BX71" s="61"/>
+      <c r="BY71" s="61"/>
       <c r="BZ71" s="47"/>
       <c r="CA71" s="47"/>
       <c r="CB71" s="49"/>
@@ -29598,17 +29468,17 @@
       <c r="CK71" s="47"/>
       <c r="CL71" s="47"/>
       <c r="CM71" s="47"/>
-      <c r="CN71" s="61"/>
-      <c r="CO71" s="64"/>
-      <c r="CP71" s="64"/>
-      <c r="CQ71" s="64"/>
-      <c r="CR71" s="64"/>
-      <c r="CS71" s="64"/>
-      <c r="CT71" s="64"/>
-      <c r="CU71" s="64"/>
-      <c r="CV71" s="62" t="s">
+      <c r="CN71" s="61" t="s">
         <v>233</v>
       </c>
+      <c r="CO71" s="61"/>
+      <c r="CP71" s="61"/>
+      <c r="CQ71" s="61"/>
+      <c r="CR71" s="61"/>
+      <c r="CS71" s="61"/>
+      <c r="CT71" s="61"/>
+      <c r="CU71" s="61"/>
+      <c r="CV71" s="61"/>
       <c r="CW71" s="47"/>
       <c r="CX71" s="47"/>
       <c r="CY71" s="47"/>
@@ -29623,17 +29493,17 @@
       <c r="DH71" s="47"/>
       <c r="DI71" s="47"/>
       <c r="DJ71" s="47"/>
-      <c r="DK71" s="61"/>
-      <c r="DL71" s="64"/>
-      <c r="DM71" s="64"/>
-      <c r="DN71" s="64"/>
-      <c r="DO71" s="64"/>
-      <c r="DP71" s="64"/>
-      <c r="DQ71" s="64"/>
-      <c r="DR71" s="64"/>
-      <c r="DS71" s="62" t="s">
+      <c r="DK71" s="61" t="s">
         <v>233</v>
       </c>
+      <c r="DL71" s="61"/>
+      <c r="DM71" s="61"/>
+      <c r="DN71" s="61"/>
+      <c r="DO71" s="61"/>
+      <c r="DP71" s="61"/>
+      <c r="DQ71" s="61"/>
+      <c r="DR71" s="61"/>
+      <c r="DS71" s="61"/>
       <c r="DT71" s="47"/>
       <c r="DU71" s="49"/>
       <c r="DV71" s="49"/>
@@ -29647,8 +29517,10 @@
       <c r="ED71" s="47"/>
       <c r="EE71" s="47"/>
     </row>
-    <row r="72" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="61"/>
+    <row r="72" customFormat="false" ht="22.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="61" t="s">
+        <v>234</v>
+      </c>
       <c r="B72" s="61"/>
       <c r="C72" s="61"/>
       <c r="D72" s="61"/>
@@ -29657,9 +29529,7 @@
       <c r="G72" s="61"/>
       <c r="H72" s="61"/>
       <c r="I72" s="61"/>
-      <c r="J72" s="62" t="s">
-        <v>234</v>
-      </c>
+      <c r="J72" s="61"/>
       <c r="K72" s="39"/>
       <c r="L72" s="49"/>
       <c r="M72" s="49"/>
@@ -29671,18 +29541,18 @@
       <c r="S72" s="47"/>
       <c r="T72" s="47"/>
       <c r="U72" s="49"/>
-      <c r="V72" s="61"/>
+      <c r="V72" s="61" t="s">
+        <v>234</v>
+      </c>
       <c r="W72" s="61"/>
-      <c r="X72" s="64"/>
-      <c r="Y72" s="64"/>
-      <c r="Z72" s="64"/>
-      <c r="AA72" s="64"/>
-      <c r="AB72" s="64"/>
-      <c r="AC72" s="64"/>
-      <c r="AD72" s="64"/>
-      <c r="AE72" s="62" t="s">
-        <v>234</v>
-      </c>
+      <c r="X72" s="61"/>
+      <c r="Y72" s="61"/>
+      <c r="Z72" s="61"/>
+      <c r="AA72" s="61"/>
+      <c r="AB72" s="61"/>
+      <c r="AC72" s="61"/>
+      <c r="AD72" s="61"/>
+      <c r="AE72" s="61"/>
       <c r="AF72" s="47"/>
       <c r="AG72" s="49"/>
       <c r="AH72" s="49"/>
@@ -29697,17 +29567,17 @@
       <c r="AQ72" s="49"/>
       <c r="AR72" s="47"/>
       <c r="AS72" s="49"/>
-      <c r="AT72" s="61"/>
-      <c r="AU72" s="64"/>
-      <c r="AV72" s="64"/>
-      <c r="AW72" s="64"/>
-      <c r="AX72" s="64"/>
-      <c r="AY72" s="64"/>
-      <c r="AZ72" s="64"/>
-      <c r="BA72" s="64"/>
-      <c r="BB72" s="62" t="s">
+      <c r="AT72" s="61" t="s">
         <v>234</v>
       </c>
+      <c r="AU72" s="61"/>
+      <c r="AV72" s="61"/>
+      <c r="AW72" s="61"/>
+      <c r="AX72" s="61"/>
+      <c r="AY72" s="61"/>
+      <c r="AZ72" s="61"/>
+      <c r="BA72" s="61"/>
+      <c r="BB72" s="61"/>
       <c r="BC72" s="49"/>
       <c r="BD72" s="47"/>
       <c r="BE72" s="49"/>
@@ -29722,17 +29592,17 @@
       <c r="BN72" s="49"/>
       <c r="BO72" s="49"/>
       <c r="BP72" s="49"/>
-      <c r="BQ72" s="61"/>
-      <c r="BR72" s="64"/>
-      <c r="BS72" s="64"/>
-      <c r="BT72" s="64"/>
-      <c r="BU72" s="64"/>
-      <c r="BV72" s="64"/>
-      <c r="BW72" s="64"/>
-      <c r="BX72" s="64"/>
-      <c r="BY72" s="62" t="s">
+      <c r="BQ72" s="61" t="s">
         <v>234</v>
       </c>
+      <c r="BR72" s="61"/>
+      <c r="BS72" s="61"/>
+      <c r="BT72" s="61"/>
+      <c r="BU72" s="61"/>
+      <c r="BV72" s="61"/>
+      <c r="BW72" s="61"/>
+      <c r="BX72" s="61"/>
+      <c r="BY72" s="61"/>
       <c r="BZ72" s="47"/>
       <c r="CA72" s="47"/>
       <c r="CB72" s="49"/>
@@ -29747,17 +29617,17 @@
       <c r="CK72" s="47"/>
       <c r="CL72" s="49"/>
       <c r="CM72" s="47"/>
-      <c r="CN72" s="61"/>
-      <c r="CO72" s="64"/>
-      <c r="CP72" s="64"/>
-      <c r="CQ72" s="64"/>
-      <c r="CR72" s="64"/>
-      <c r="CS72" s="64"/>
-      <c r="CT72" s="64"/>
-      <c r="CU72" s="64"/>
-      <c r="CV72" s="62" t="s">
+      <c r="CN72" s="61" t="s">
         <v>234</v>
       </c>
+      <c r="CO72" s="61"/>
+      <c r="CP72" s="61"/>
+      <c r="CQ72" s="61"/>
+      <c r="CR72" s="61"/>
+      <c r="CS72" s="61"/>
+      <c r="CT72" s="61"/>
+      <c r="CU72" s="61"/>
+      <c r="CV72" s="61"/>
       <c r="CW72" s="47"/>
       <c r="CX72" s="47"/>
       <c r="CY72" s="47"/>
@@ -29772,17 +29642,17 @@
       <c r="DH72" s="49"/>
       <c r="DI72" s="47"/>
       <c r="DJ72" s="47"/>
-      <c r="DK72" s="61"/>
-      <c r="DL72" s="64"/>
-      <c r="DM72" s="64"/>
-      <c r="DN72" s="64"/>
-      <c r="DO72" s="64"/>
-      <c r="DP72" s="64"/>
-      <c r="DQ72" s="64"/>
-      <c r="DR72" s="64"/>
-      <c r="DS72" s="62" t="s">
+      <c r="DK72" s="61" t="s">
         <v>234</v>
       </c>
+      <c r="DL72" s="61"/>
+      <c r="DM72" s="61"/>
+      <c r="DN72" s="61"/>
+      <c r="DO72" s="61"/>
+      <c r="DP72" s="61"/>
+      <c r="DQ72" s="61"/>
+      <c r="DR72" s="61"/>
+      <c r="DS72" s="61"/>
       <c r="DT72" s="47"/>
       <c r="DU72" s="49"/>
       <c r="DV72" s="49"/>
@@ -29796,8 +29666,10 @@
       <c r="ED72" s="47"/>
       <c r="EE72" s="47"/>
     </row>
-    <row r="73" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="61"/>
+    <row r="73" customFormat="false" ht="26.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="61" t="s">
+        <v>235</v>
+      </c>
       <c r="B73" s="61"/>
       <c r="C73" s="61"/>
       <c r="D73" s="61"/>
@@ -29806,46 +29678,44 @@
       <c r="G73" s="61"/>
       <c r="H73" s="61"/>
       <c r="I73" s="61"/>
-      <c r="J73" s="67" t="s">
+      <c r="J73" s="61"/>
+      <c r="K73" s="65"/>
+      <c r="L73" s="65"/>
+      <c r="M73" s="65"/>
+      <c r="N73" s="65"/>
+      <c r="O73" s="65"/>
+      <c r="P73" s="65"/>
+      <c r="Q73" s="65"/>
+      <c r="R73" s="65"/>
+      <c r="S73" s="65"/>
+      <c r="T73" s="65"/>
+      <c r="U73" s="65"/>
+      <c r="V73" s="61" t="s">
         <v>235</v>
       </c>
-      <c r="K73" s="68"/>
-      <c r="L73" s="68"/>
-      <c r="M73" s="68"/>
-      <c r="N73" s="68"/>
-      <c r="O73" s="68"/>
-      <c r="P73" s="68"/>
-      <c r="Q73" s="68"/>
-      <c r="R73" s="68"/>
-      <c r="S73" s="68"/>
-      <c r="T73" s="68"/>
-      <c r="U73" s="68"/>
-      <c r="V73" s="67" t="s">
-        <v>235</v>
-      </c>
-      <c r="W73" s="67"/>
-      <c r="X73" s="67"/>
-      <c r="Y73" s="67"/>
-      <c r="Z73" s="67"/>
-      <c r="AA73" s="67"/>
-      <c r="AB73" s="67"/>
-      <c r="AC73" s="67"/>
-      <c r="AD73" s="67"/>
-      <c r="AE73" s="67"/>
-      <c r="AF73" s="69"/>
-      <c r="AG73" s="69"/>
-      <c r="AH73" s="69"/>
-      <c r="AI73" s="69"/>
-      <c r="AJ73" s="69"/>
-      <c r="AK73" s="69"/>
-      <c r="AL73" s="69"/>
-      <c r="AM73" s="69"/>
-      <c r="AN73" s="69"/>
-      <c r="AO73" s="69"/>
-      <c r="AP73" s="69"/>
-      <c r="AQ73" s="69"/>
-      <c r="AR73" s="69"/>
-      <c r="AS73" s="69"/>
+      <c r="W73" s="61"/>
+      <c r="X73" s="61"/>
+      <c r="Y73" s="61"/>
+      <c r="Z73" s="61"/>
+      <c r="AA73" s="61"/>
+      <c r="AB73" s="61"/>
+      <c r="AC73" s="61"/>
+      <c r="AD73" s="61"/>
+      <c r="AE73" s="61"/>
+      <c r="AF73" s="66"/>
+      <c r="AG73" s="66"/>
+      <c r="AH73" s="66"/>
+      <c r="AI73" s="66"/>
+      <c r="AJ73" s="66"/>
+      <c r="AK73" s="66"/>
+      <c r="AL73" s="66"/>
+      <c r="AM73" s="66"/>
+      <c r="AN73" s="66"/>
+      <c r="AO73" s="66"/>
+      <c r="AP73" s="66"/>
+      <c r="AQ73" s="66"/>
+      <c r="AR73" s="66"/>
+      <c r="AS73" s="66"/>
       <c r="AT73" s="67" t="s">
         <v>235</v>
       </c>
@@ -29857,20 +29727,20 @@
       <c r="AZ73" s="67"/>
       <c r="BA73" s="67"/>
       <c r="BB73" s="67"/>
-      <c r="BC73" s="70"/>
-      <c r="BD73" s="70"/>
-      <c r="BE73" s="70"/>
-      <c r="BF73" s="70"/>
-      <c r="BG73" s="70"/>
-      <c r="BH73" s="70"/>
-      <c r="BI73" s="70"/>
-      <c r="BJ73" s="70"/>
-      <c r="BK73" s="70"/>
-      <c r="BL73" s="70"/>
-      <c r="BM73" s="70"/>
-      <c r="BN73" s="70"/>
-      <c r="BO73" s="70"/>
-      <c r="BP73" s="70"/>
+      <c r="BC73" s="66"/>
+      <c r="BD73" s="66"/>
+      <c r="BE73" s="66"/>
+      <c r="BF73" s="66"/>
+      <c r="BG73" s="66"/>
+      <c r="BH73" s="66"/>
+      <c r="BI73" s="66"/>
+      <c r="BJ73" s="66"/>
+      <c r="BK73" s="66"/>
+      <c r="BL73" s="66"/>
+      <c r="BM73" s="66"/>
+      <c r="BN73" s="66"/>
+      <c r="BO73" s="66"/>
+      <c r="BP73" s="66"/>
       <c r="BQ73" s="67" t="s">
         <v>235</v>
       </c>
@@ -29882,20 +29752,20 @@
       <c r="BW73" s="67"/>
       <c r="BX73" s="67"/>
       <c r="BY73" s="67"/>
-      <c r="BZ73" s="68"/>
-      <c r="CA73" s="68"/>
-      <c r="CB73" s="68"/>
-      <c r="CC73" s="68"/>
-      <c r="CD73" s="68"/>
-      <c r="CE73" s="68"/>
-      <c r="CF73" s="68"/>
-      <c r="CG73" s="68"/>
-      <c r="CH73" s="68"/>
-      <c r="CI73" s="68"/>
-      <c r="CJ73" s="68"/>
-      <c r="CK73" s="68"/>
-      <c r="CL73" s="68"/>
-      <c r="CM73" s="68"/>
+      <c r="BZ73" s="65"/>
+      <c r="CA73" s="65"/>
+      <c r="CB73" s="65"/>
+      <c r="CC73" s="65"/>
+      <c r="CD73" s="65"/>
+      <c r="CE73" s="65"/>
+      <c r="CF73" s="65"/>
+      <c r="CG73" s="65"/>
+      <c r="CH73" s="65"/>
+      <c r="CI73" s="65"/>
+      <c r="CJ73" s="65"/>
+      <c r="CK73" s="65"/>
+      <c r="CL73" s="65"/>
+      <c r="CM73" s="65"/>
       <c r="CN73" s="67" t="s">
         <v>235</v>
       </c>
@@ -29907,20 +29777,20 @@
       <c r="CT73" s="67"/>
       <c r="CU73" s="67"/>
       <c r="CV73" s="67"/>
-      <c r="CW73" s="71"/>
-      <c r="CX73" s="71"/>
-      <c r="CY73" s="71"/>
-      <c r="CZ73" s="71"/>
-      <c r="DA73" s="71"/>
-      <c r="DB73" s="71"/>
-      <c r="DC73" s="71"/>
-      <c r="DD73" s="71"/>
-      <c r="DE73" s="71"/>
-      <c r="DF73" s="71"/>
-      <c r="DG73" s="71"/>
-      <c r="DH73" s="71"/>
-      <c r="DI73" s="71"/>
-      <c r="DJ73" s="71"/>
+      <c r="CW73" s="65"/>
+      <c r="CX73" s="65"/>
+      <c r="CY73" s="65"/>
+      <c r="CZ73" s="65"/>
+      <c r="DA73" s="65"/>
+      <c r="DB73" s="65"/>
+      <c r="DC73" s="65"/>
+      <c r="DD73" s="65"/>
+      <c r="DE73" s="65"/>
+      <c r="DF73" s="65"/>
+      <c r="DG73" s="65"/>
+      <c r="DH73" s="65"/>
+      <c r="DI73" s="65"/>
+      <c r="DJ73" s="65"/>
       <c r="DK73" s="67" t="s">
         <v>235</v>
       </c>
@@ -29932,21 +29802,23 @@
       <c r="DQ73" s="67"/>
       <c r="DR73" s="67"/>
       <c r="DS73" s="67"/>
-      <c r="DT73" s="68"/>
-      <c r="DU73" s="68"/>
-      <c r="DV73" s="68"/>
-      <c r="DW73" s="68"/>
-      <c r="DX73" s="68"/>
-      <c r="DY73" s="68"/>
-      <c r="DZ73" s="68"/>
-      <c r="EA73" s="68"/>
-      <c r="EB73" s="68"/>
-      <c r="EC73" s="68"/>
-      <c r="ED73" s="68"/>
-      <c r="EE73" s="68"/>
+      <c r="DT73" s="65"/>
+      <c r="DU73" s="65"/>
+      <c r="DV73" s="65"/>
+      <c r="DW73" s="65"/>
+      <c r="DX73" s="65"/>
+      <c r="DY73" s="65"/>
+      <c r="DZ73" s="65"/>
+      <c r="EA73" s="65"/>
+      <c r="EB73" s="65"/>
+      <c r="EC73" s="65"/>
+      <c r="ED73" s="65"/>
+      <c r="EE73" s="65"/>
     </row>
-    <row r="74" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="61"/>
+    <row r="74" customFormat="false" ht="26.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="61" t="s">
+        <v>236</v>
+      </c>
       <c r="B74" s="61"/>
       <c r="C74" s="61"/>
       <c r="D74" s="61"/>
@@ -29955,47 +29827,47 @@
       <c r="G74" s="61"/>
       <c r="H74" s="61"/>
       <c r="I74" s="61"/>
-      <c r="J74" s="67" t="s">
+      <c r="J74" s="61"/>
+      <c r="K74" s="65"/>
+      <c r="L74" s="65"/>
+      <c r="M74" s="65"/>
+      <c r="N74" s="65"/>
+      <c r="O74" s="65"/>
+      <c r="P74" s="65"/>
+      <c r="Q74" s="65"/>
+      <c r="R74" s="65"/>
+      <c r="S74" s="65"/>
+      <c r="T74" s="65"/>
+      <c r="U74" s="65"/>
+      <c r="V74" s="61" t="s">
         <v>236</v>
       </c>
-      <c r="K74" s="68"/>
-      <c r="L74" s="68"/>
-      <c r="M74" s="68"/>
-      <c r="N74" s="68"/>
-      <c r="O74" s="68"/>
-      <c r="P74" s="68"/>
-      <c r="Q74" s="68"/>
-      <c r="R74" s="68"/>
-      <c r="S74" s="68"/>
-      <c r="T74" s="68"/>
-      <c r="U74" s="68"/>
-      <c r="V74" s="67"/>
-      <c r="W74" s="67"/>
-      <c r="X74" s="67"/>
-      <c r="Y74" s="67"/>
-      <c r="Z74" s="67"/>
-      <c r="AA74" s="67"/>
-      <c r="AB74" s="67"/>
-      <c r="AC74" s="67"/>
-      <c r="AD74" s="67"/>
-      <c r="AE74" s="67" t="s">
+      <c r="W74" s="61"/>
+      <c r="X74" s="61"/>
+      <c r="Y74" s="61"/>
+      <c r="Z74" s="61"/>
+      <c r="AA74" s="61"/>
+      <c r="AB74" s="61"/>
+      <c r="AC74" s="61"/>
+      <c r="AD74" s="61"/>
+      <c r="AE74" s="61"/>
+      <c r="AF74" s="66"/>
+      <c r="AG74" s="66"/>
+      <c r="AH74" s="66"/>
+      <c r="AI74" s="66"/>
+      <c r="AJ74" s="66"/>
+      <c r="AK74" s="66"/>
+      <c r="AL74" s="66"/>
+      <c r="AM74" s="66"/>
+      <c r="AN74" s="66"/>
+      <c r="AO74" s="66"/>
+      <c r="AP74" s="66"/>
+      <c r="AQ74" s="66"/>
+      <c r="AR74" s="66"/>
+      <c r="AS74" s="66"/>
+      <c r="AT74" s="67" t="s">
         <v>236</v>
       </c>
-      <c r="AF74" s="69"/>
-      <c r="AG74" s="69"/>
-      <c r="AH74" s="69"/>
-      <c r="AI74" s="69"/>
-      <c r="AJ74" s="69"/>
-      <c r="AK74" s="69"/>
-      <c r="AL74" s="69"/>
-      <c r="AM74" s="69"/>
-      <c r="AN74" s="69"/>
-      <c r="AO74" s="69"/>
-      <c r="AP74" s="69"/>
-      <c r="AQ74" s="69"/>
-      <c r="AR74" s="69"/>
-      <c r="AS74" s="69"/>
-      <c r="AT74" s="67"/>
       <c r="AU74" s="67"/>
       <c r="AV74" s="67"/>
       <c r="AW74" s="67"/>
@@ -30003,24 +29875,24 @@
       <c r="AY74" s="67"/>
       <c r="AZ74" s="67"/>
       <c r="BA74" s="67"/>
-      <c r="BB74" s="67" t="s">
+      <c r="BB74" s="67"/>
+      <c r="BC74" s="66"/>
+      <c r="BD74" s="66"/>
+      <c r="BE74" s="66"/>
+      <c r="BF74" s="66"/>
+      <c r="BG74" s="66"/>
+      <c r="BH74" s="66"/>
+      <c r="BI74" s="66"/>
+      <c r="BJ74" s="66"/>
+      <c r="BK74" s="66"/>
+      <c r="BL74" s="66"/>
+      <c r="BM74" s="66"/>
+      <c r="BN74" s="66"/>
+      <c r="BO74" s="66"/>
+      <c r="BP74" s="66"/>
+      <c r="BQ74" s="67" t="s">
         <v>236</v>
       </c>
-      <c r="BC74" s="70"/>
-      <c r="BD74" s="70"/>
-      <c r="BE74" s="70"/>
-      <c r="BF74" s="70"/>
-      <c r="BG74" s="70"/>
-      <c r="BH74" s="70"/>
-      <c r="BI74" s="70"/>
-      <c r="BJ74" s="70"/>
-      <c r="BK74" s="70"/>
-      <c r="BL74" s="70"/>
-      <c r="BM74" s="70"/>
-      <c r="BN74" s="70"/>
-      <c r="BO74" s="70"/>
-      <c r="BP74" s="70"/>
-      <c r="BQ74" s="67"/>
       <c r="BR74" s="67"/>
       <c r="BS74" s="67"/>
       <c r="BT74" s="67"/>
@@ -30028,24 +29900,24 @@
       <c r="BV74" s="67"/>
       <c r="BW74" s="67"/>
       <c r="BX74" s="67"/>
-      <c r="BY74" s="67" t="s">
+      <c r="BY74" s="67"/>
+      <c r="BZ74" s="65"/>
+      <c r="CA74" s="65"/>
+      <c r="CB74" s="65"/>
+      <c r="CC74" s="65"/>
+      <c r="CD74" s="65"/>
+      <c r="CE74" s="65"/>
+      <c r="CF74" s="65"/>
+      <c r="CG74" s="65"/>
+      <c r="CH74" s="65"/>
+      <c r="CI74" s="65"/>
+      <c r="CJ74" s="65"/>
+      <c r="CK74" s="65"/>
+      <c r="CL74" s="65"/>
+      <c r="CM74" s="65"/>
+      <c r="CN74" s="67" t="s">
         <v>236</v>
       </c>
-      <c r="BZ74" s="68"/>
-      <c r="CA74" s="68"/>
-      <c r="CB74" s="68"/>
-      <c r="CC74" s="68"/>
-      <c r="CD74" s="68"/>
-      <c r="CE74" s="68"/>
-      <c r="CF74" s="68"/>
-      <c r="CG74" s="68"/>
-      <c r="CH74" s="68"/>
-      <c r="CI74" s="68"/>
-      <c r="CJ74" s="68"/>
-      <c r="CK74" s="68"/>
-      <c r="CL74" s="68"/>
-      <c r="CM74" s="68"/>
-      <c r="CN74" s="67"/>
       <c r="CO74" s="67"/>
       <c r="CP74" s="67"/>
       <c r="CQ74" s="67"/>
@@ -30053,24 +29925,24 @@
       <c r="CS74" s="67"/>
       <c r="CT74" s="67"/>
       <c r="CU74" s="67"/>
-      <c r="CV74" s="67" t="s">
+      <c r="CV74" s="67"/>
+      <c r="CW74" s="65"/>
+      <c r="CX74" s="65"/>
+      <c r="CY74" s="65"/>
+      <c r="CZ74" s="65"/>
+      <c r="DA74" s="65"/>
+      <c r="DB74" s="65"/>
+      <c r="DC74" s="65"/>
+      <c r="DD74" s="65"/>
+      <c r="DE74" s="65"/>
+      <c r="DF74" s="65"/>
+      <c r="DG74" s="65"/>
+      <c r="DH74" s="65"/>
+      <c r="DI74" s="65"/>
+      <c r="DJ74" s="65"/>
+      <c r="DK74" s="67" t="s">
         <v>236</v>
       </c>
-      <c r="CW74" s="71"/>
-      <c r="CX74" s="71"/>
-      <c r="CY74" s="71"/>
-      <c r="CZ74" s="71"/>
-      <c r="DA74" s="71"/>
-      <c r="DB74" s="71"/>
-      <c r="DC74" s="71"/>
-      <c r="DD74" s="71"/>
-      <c r="DE74" s="71"/>
-      <c r="DF74" s="71"/>
-      <c r="DG74" s="71"/>
-      <c r="DH74" s="71"/>
-      <c r="DI74" s="71"/>
-      <c r="DJ74" s="71"/>
-      <c r="DK74" s="67"/>
       <c r="DL74" s="67"/>
       <c r="DM74" s="67"/>
       <c r="DN74" s="67"/>
@@ -30078,24 +29950,24 @@
       <c r="DP74" s="67"/>
       <c r="DQ74" s="67"/>
       <c r="DR74" s="67"/>
-      <c r="DS74" s="67" t="s">
-        <v>236</v>
-      </c>
-      <c r="DT74" s="68"/>
-      <c r="DU74" s="68"/>
-      <c r="DV74" s="68"/>
-      <c r="DW74" s="68"/>
-      <c r="DX74" s="68"/>
-      <c r="DY74" s="68"/>
-      <c r="DZ74" s="68"/>
-      <c r="EA74" s="68"/>
-      <c r="EB74" s="68"/>
-      <c r="EC74" s="68"/>
-      <c r="ED74" s="68"/>
-      <c r="EE74" s="68"/>
+      <c r="DS74" s="67"/>
+      <c r="DT74" s="65"/>
+      <c r="DU74" s="65"/>
+      <c r="DV74" s="65"/>
+      <c r="DW74" s="65"/>
+      <c r="DX74" s="65"/>
+      <c r="DY74" s="65"/>
+      <c r="DZ74" s="65"/>
+      <c r="EA74" s="65"/>
+      <c r="EB74" s="65"/>
+      <c r="EC74" s="65"/>
+      <c r="ED74" s="65"/>
+      <c r="EE74" s="65"/>
     </row>
-    <row r="75" customFormat="false" ht="31.15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="61"/>
+    <row r="75" customFormat="false" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="61" t="s">
+        <v>237</v>
+      </c>
       <c r="B75" s="61"/>
       <c r="C75" s="61"/>
       <c r="D75" s="61"/>
@@ -30104,47 +29976,47 @@
       <c r="G75" s="61"/>
       <c r="H75" s="61"/>
       <c r="I75" s="61"/>
-      <c r="J75" s="67" t="s">
+      <c r="J75" s="61"/>
+      <c r="K75" s="65"/>
+      <c r="L75" s="65"/>
+      <c r="M75" s="65"/>
+      <c r="N75" s="65"/>
+      <c r="O75" s="65"/>
+      <c r="P75" s="65"/>
+      <c r="Q75" s="65"/>
+      <c r="R75" s="65"/>
+      <c r="S75" s="65"/>
+      <c r="T75" s="65"/>
+      <c r="U75" s="65"/>
+      <c r="V75" s="61" t="s">
         <v>237</v>
       </c>
-      <c r="K75" s="68"/>
-      <c r="L75" s="68"/>
-      <c r="M75" s="68"/>
-      <c r="N75" s="68"/>
-      <c r="O75" s="68"/>
-      <c r="P75" s="68"/>
-      <c r="Q75" s="68"/>
-      <c r="R75" s="68"/>
-      <c r="S75" s="68"/>
-      <c r="T75" s="68"/>
-      <c r="U75" s="68"/>
-      <c r="V75" s="67"/>
-      <c r="W75" s="67"/>
-      <c r="X75" s="67"/>
-      <c r="Y75" s="67"/>
-      <c r="Z75" s="67"/>
-      <c r="AA75" s="67"/>
-      <c r="AB75" s="67"/>
-      <c r="AC75" s="67"/>
-      <c r="AD75" s="67"/>
-      <c r="AE75" s="67" t="s">
+      <c r="W75" s="61"/>
+      <c r="X75" s="61"/>
+      <c r="Y75" s="61"/>
+      <c r="Z75" s="61"/>
+      <c r="AA75" s="61"/>
+      <c r="AB75" s="61"/>
+      <c r="AC75" s="61"/>
+      <c r="AD75" s="61"/>
+      <c r="AE75" s="61"/>
+      <c r="AF75" s="66"/>
+      <c r="AG75" s="66"/>
+      <c r="AH75" s="66"/>
+      <c r="AI75" s="66"/>
+      <c r="AJ75" s="66"/>
+      <c r="AK75" s="66"/>
+      <c r="AL75" s="66"/>
+      <c r="AM75" s="66"/>
+      <c r="AN75" s="66"/>
+      <c r="AO75" s="66"/>
+      <c r="AP75" s="66"/>
+      <c r="AQ75" s="66"/>
+      <c r="AR75" s="66"/>
+      <c r="AS75" s="66"/>
+      <c r="AT75" s="67" t="s">
         <v>237</v>
       </c>
-      <c r="AF75" s="69"/>
-      <c r="AG75" s="69"/>
-      <c r="AH75" s="69"/>
-      <c r="AI75" s="69"/>
-      <c r="AJ75" s="69"/>
-      <c r="AK75" s="69"/>
-      <c r="AL75" s="69"/>
-      <c r="AM75" s="69"/>
-      <c r="AN75" s="69"/>
-      <c r="AO75" s="69"/>
-      <c r="AP75" s="69"/>
-      <c r="AQ75" s="69"/>
-      <c r="AR75" s="69"/>
-      <c r="AS75" s="69"/>
-      <c r="AT75" s="67"/>
       <c r="AU75" s="67"/>
       <c r="AV75" s="67"/>
       <c r="AW75" s="67"/>
@@ -30152,24 +30024,24 @@
       <c r="AY75" s="67"/>
       <c r="AZ75" s="67"/>
       <c r="BA75" s="67"/>
-      <c r="BB75" s="67" t="s">
+      <c r="BB75" s="67"/>
+      <c r="BC75" s="66"/>
+      <c r="BD75" s="66"/>
+      <c r="BE75" s="66"/>
+      <c r="BF75" s="66"/>
+      <c r="BG75" s="66"/>
+      <c r="BH75" s="66"/>
+      <c r="BI75" s="66"/>
+      <c r="BJ75" s="66"/>
+      <c r="BK75" s="66"/>
+      <c r="BL75" s="66"/>
+      <c r="BM75" s="66"/>
+      <c r="BN75" s="66"/>
+      <c r="BO75" s="66"/>
+      <c r="BP75" s="66"/>
+      <c r="BQ75" s="67" t="s">
         <v>237</v>
       </c>
-      <c r="BC75" s="70"/>
-      <c r="BD75" s="70"/>
-      <c r="BE75" s="70"/>
-      <c r="BF75" s="70"/>
-      <c r="BG75" s="70"/>
-      <c r="BH75" s="70"/>
-      <c r="BI75" s="70"/>
-      <c r="BJ75" s="70"/>
-      <c r="BK75" s="70"/>
-      <c r="BL75" s="70"/>
-      <c r="BM75" s="70"/>
-      <c r="BN75" s="70"/>
-      <c r="BO75" s="70"/>
-      <c r="BP75" s="70"/>
-      <c r="BQ75" s="67"/>
       <c r="BR75" s="67"/>
       <c r="BS75" s="67"/>
       <c r="BT75" s="67"/>
@@ -30177,24 +30049,24 @@
       <c r="BV75" s="67"/>
       <c r="BW75" s="67"/>
       <c r="BX75" s="67"/>
-      <c r="BY75" s="67" t="s">
+      <c r="BY75" s="67"/>
+      <c r="BZ75" s="65"/>
+      <c r="CA75" s="65"/>
+      <c r="CB75" s="65"/>
+      <c r="CC75" s="65"/>
+      <c r="CD75" s="65"/>
+      <c r="CE75" s="65"/>
+      <c r="CF75" s="65"/>
+      <c r="CG75" s="65"/>
+      <c r="CH75" s="65"/>
+      <c r="CI75" s="65"/>
+      <c r="CJ75" s="65"/>
+      <c r="CK75" s="65"/>
+      <c r="CL75" s="65"/>
+      <c r="CM75" s="65"/>
+      <c r="CN75" s="67" t="s">
         <v>237</v>
       </c>
-      <c r="BZ75" s="68"/>
-      <c r="CA75" s="68"/>
-      <c r="CB75" s="68"/>
-      <c r="CC75" s="68"/>
-      <c r="CD75" s="68"/>
-      <c r="CE75" s="68"/>
-      <c r="CF75" s="68"/>
-      <c r="CG75" s="68"/>
-      <c r="CH75" s="68"/>
-      <c r="CI75" s="68"/>
-      <c r="CJ75" s="68"/>
-      <c r="CK75" s="68"/>
-      <c r="CL75" s="68"/>
-      <c r="CM75" s="68"/>
-      <c r="CN75" s="67"/>
       <c r="CO75" s="67"/>
       <c r="CP75" s="67"/>
       <c r="CQ75" s="67"/>
@@ -30202,24 +30074,24 @@
       <c r="CS75" s="67"/>
       <c r="CT75" s="67"/>
       <c r="CU75" s="67"/>
-      <c r="CV75" s="67" t="s">
+      <c r="CV75" s="67"/>
+      <c r="CW75" s="65"/>
+      <c r="CX75" s="65"/>
+      <c r="CY75" s="65"/>
+      <c r="CZ75" s="65"/>
+      <c r="DA75" s="65"/>
+      <c r="DB75" s="65"/>
+      <c r="DC75" s="65"/>
+      <c r="DD75" s="65"/>
+      <c r="DE75" s="65"/>
+      <c r="DF75" s="65"/>
+      <c r="DG75" s="65"/>
+      <c r="DH75" s="65"/>
+      <c r="DI75" s="65"/>
+      <c r="DJ75" s="65"/>
+      <c r="DK75" s="67" t="s">
         <v>237</v>
       </c>
-      <c r="CW75" s="71"/>
-      <c r="CX75" s="71"/>
-      <c r="CY75" s="71"/>
-      <c r="CZ75" s="71"/>
-      <c r="DA75" s="71"/>
-      <c r="DB75" s="71"/>
-      <c r="DC75" s="71"/>
-      <c r="DD75" s="71"/>
-      <c r="DE75" s="71"/>
-      <c r="DF75" s="71"/>
-      <c r="DG75" s="71"/>
-      <c r="DH75" s="71"/>
-      <c r="DI75" s="71"/>
-      <c r="DJ75" s="71"/>
-      <c r="DK75" s="67"/>
       <c r="DL75" s="67"/>
       <c r="DM75" s="67"/>
       <c r="DN75" s="67"/>
@@ -30227,24 +30099,24 @@
       <c r="DP75" s="67"/>
       <c r="DQ75" s="67"/>
       <c r="DR75" s="67"/>
-      <c r="DS75" s="67" t="s">
-        <v>237</v>
-      </c>
-      <c r="DT75" s="68"/>
-      <c r="DU75" s="68"/>
-      <c r="DV75" s="68"/>
-      <c r="DW75" s="68"/>
-      <c r="DX75" s="68"/>
-      <c r="DY75" s="68"/>
-      <c r="DZ75" s="68"/>
-      <c r="EA75" s="68"/>
-      <c r="EB75" s="68"/>
-      <c r="EC75" s="68"/>
-      <c r="ED75" s="68"/>
-      <c r="EE75" s="68"/>
+      <c r="DS75" s="67"/>
+      <c r="DT75" s="65"/>
+      <c r="DU75" s="65"/>
+      <c r="DV75" s="65"/>
+      <c r="DW75" s="65"/>
+      <c r="DX75" s="65"/>
+      <c r="DY75" s="65"/>
+      <c r="DZ75" s="65"/>
+      <c r="EA75" s="65"/>
+      <c r="EB75" s="65"/>
+      <c r="EC75" s="65"/>
+      <c r="ED75" s="65"/>
+      <c r="EE75" s="65"/>
     </row>
-    <row r="76" customFormat="false" ht="54" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="61"/>
+    <row r="76" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="61" t="s">
+        <v>238</v>
+      </c>
       <c r="B76" s="61"/>
       <c r="C76" s="61"/>
       <c r="D76" s="61"/>
@@ -30253,47 +30125,47 @@
       <c r="G76" s="61"/>
       <c r="H76" s="61"/>
       <c r="I76" s="61"/>
-      <c r="J76" s="67" t="s">
+      <c r="J76" s="61"/>
+      <c r="K76" s="65"/>
+      <c r="L76" s="65"/>
+      <c r="M76" s="65"/>
+      <c r="N76" s="65"/>
+      <c r="O76" s="65"/>
+      <c r="P76" s="65"/>
+      <c r="Q76" s="65"/>
+      <c r="R76" s="65"/>
+      <c r="S76" s="65"/>
+      <c r="T76" s="65"/>
+      <c r="U76" s="65"/>
+      <c r="V76" s="61" t="s">
         <v>238</v>
       </c>
-      <c r="K76" s="68"/>
-      <c r="L76" s="68"/>
-      <c r="M76" s="68"/>
-      <c r="N76" s="68"/>
-      <c r="O76" s="68"/>
-      <c r="P76" s="68"/>
-      <c r="Q76" s="68"/>
-      <c r="R76" s="68"/>
-      <c r="S76" s="68"/>
-      <c r="T76" s="68"/>
-      <c r="U76" s="68"/>
-      <c r="V76" s="67"/>
-      <c r="W76" s="67"/>
-      <c r="X76" s="67"/>
-      <c r="Y76" s="67"/>
-      <c r="Z76" s="67"/>
-      <c r="AA76" s="67"/>
-      <c r="AB76" s="67"/>
-      <c r="AC76" s="67"/>
-      <c r="AD76" s="67"/>
-      <c r="AE76" s="67" t="s">
+      <c r="W76" s="61"/>
+      <c r="X76" s="61"/>
+      <c r="Y76" s="61"/>
+      <c r="Z76" s="61"/>
+      <c r="AA76" s="61"/>
+      <c r="AB76" s="61"/>
+      <c r="AC76" s="61"/>
+      <c r="AD76" s="61"/>
+      <c r="AE76" s="61"/>
+      <c r="AF76" s="66"/>
+      <c r="AG76" s="66"/>
+      <c r="AH76" s="66"/>
+      <c r="AI76" s="66"/>
+      <c r="AJ76" s="66"/>
+      <c r="AK76" s="66"/>
+      <c r="AL76" s="66"/>
+      <c r="AM76" s="66"/>
+      <c r="AN76" s="66"/>
+      <c r="AO76" s="66"/>
+      <c r="AP76" s="66"/>
+      <c r="AQ76" s="66"/>
+      <c r="AR76" s="66"/>
+      <c r="AS76" s="66"/>
+      <c r="AT76" s="67" t="s">
         <v>238</v>
       </c>
-      <c r="AF76" s="69"/>
-      <c r="AG76" s="69"/>
-      <c r="AH76" s="69"/>
-      <c r="AI76" s="69"/>
-      <c r="AJ76" s="69"/>
-      <c r="AK76" s="69"/>
-      <c r="AL76" s="69"/>
-      <c r="AM76" s="69"/>
-      <c r="AN76" s="69"/>
-      <c r="AO76" s="69"/>
-      <c r="AP76" s="69"/>
-      <c r="AQ76" s="69"/>
-      <c r="AR76" s="69"/>
-      <c r="AS76" s="69"/>
-      <c r="AT76" s="67"/>
       <c r="AU76" s="67"/>
       <c r="AV76" s="67"/>
       <c r="AW76" s="67"/>
@@ -30301,24 +30173,24 @@
       <c r="AY76" s="67"/>
       <c r="AZ76" s="67"/>
       <c r="BA76" s="67"/>
-      <c r="BB76" s="67" t="s">
+      <c r="BB76" s="67"/>
+      <c r="BC76" s="66"/>
+      <c r="BD76" s="66"/>
+      <c r="BE76" s="66"/>
+      <c r="BF76" s="66"/>
+      <c r="BG76" s="66"/>
+      <c r="BH76" s="66"/>
+      <c r="BI76" s="66"/>
+      <c r="BJ76" s="66"/>
+      <c r="BK76" s="66"/>
+      <c r="BL76" s="66"/>
+      <c r="BM76" s="66"/>
+      <c r="BN76" s="66"/>
+      <c r="BO76" s="66"/>
+      <c r="BP76" s="66"/>
+      <c r="BQ76" s="67" t="s">
         <v>238</v>
       </c>
-      <c r="BC76" s="70"/>
-      <c r="BD76" s="70"/>
-      <c r="BE76" s="70"/>
-      <c r="BF76" s="70"/>
-      <c r="BG76" s="70"/>
-      <c r="BH76" s="70"/>
-      <c r="BI76" s="70"/>
-      <c r="BJ76" s="70"/>
-      <c r="BK76" s="70"/>
-      <c r="BL76" s="70"/>
-      <c r="BM76" s="70"/>
-      <c r="BN76" s="70"/>
-      <c r="BO76" s="70"/>
-      <c r="BP76" s="70"/>
-      <c r="BQ76" s="67"/>
       <c r="BR76" s="67"/>
       <c r="BS76" s="67"/>
       <c r="BT76" s="67"/>
@@ -30326,24 +30198,24 @@
       <c r="BV76" s="67"/>
       <c r="BW76" s="67"/>
       <c r="BX76" s="67"/>
-      <c r="BY76" s="67" t="s">
+      <c r="BY76" s="67"/>
+      <c r="BZ76" s="65"/>
+      <c r="CA76" s="65"/>
+      <c r="CB76" s="65"/>
+      <c r="CC76" s="65"/>
+      <c r="CD76" s="65"/>
+      <c r="CE76" s="65"/>
+      <c r="CF76" s="65"/>
+      <c r="CG76" s="65"/>
+      <c r="CH76" s="65"/>
+      <c r="CI76" s="65"/>
+      <c r="CJ76" s="65"/>
+      <c r="CK76" s="65"/>
+      <c r="CL76" s="65"/>
+      <c r="CM76" s="65"/>
+      <c r="CN76" s="67" t="s">
         <v>238</v>
       </c>
-      <c r="BZ76" s="68"/>
-      <c r="CA76" s="68"/>
-      <c r="CB76" s="68"/>
-      <c r="CC76" s="68"/>
-      <c r="CD76" s="68"/>
-      <c r="CE76" s="68"/>
-      <c r="CF76" s="68"/>
-      <c r="CG76" s="68"/>
-      <c r="CH76" s="68"/>
-      <c r="CI76" s="68"/>
-      <c r="CJ76" s="68"/>
-      <c r="CK76" s="68"/>
-      <c r="CL76" s="68"/>
-      <c r="CM76" s="68"/>
-      <c r="CN76" s="67"/>
       <c r="CO76" s="67"/>
       <c r="CP76" s="67"/>
       <c r="CQ76" s="67"/>
@@ -30351,24 +30223,24 @@
       <c r="CS76" s="67"/>
       <c r="CT76" s="67"/>
       <c r="CU76" s="67"/>
-      <c r="CV76" s="67" t="s">
+      <c r="CV76" s="67"/>
+      <c r="CW76" s="65"/>
+      <c r="CX76" s="65"/>
+      <c r="CY76" s="65"/>
+      <c r="CZ76" s="65"/>
+      <c r="DA76" s="65"/>
+      <c r="DB76" s="65"/>
+      <c r="DC76" s="65"/>
+      <c r="DD76" s="65"/>
+      <c r="DE76" s="65"/>
+      <c r="DF76" s="65"/>
+      <c r="DG76" s="65"/>
+      <c r="DH76" s="65"/>
+      <c r="DI76" s="65"/>
+      <c r="DJ76" s="65"/>
+      <c r="DK76" s="67" t="s">
         <v>238</v>
       </c>
-      <c r="CW76" s="71"/>
-      <c r="CX76" s="71"/>
-      <c r="CY76" s="71"/>
-      <c r="CZ76" s="71"/>
-      <c r="DA76" s="71"/>
-      <c r="DB76" s="71"/>
-      <c r="DC76" s="71"/>
-      <c r="DD76" s="71"/>
-      <c r="DE76" s="71"/>
-      <c r="DF76" s="71"/>
-      <c r="DG76" s="71"/>
-      <c r="DH76" s="71"/>
-      <c r="DI76" s="71"/>
-      <c r="DJ76" s="71"/>
-      <c r="DK76" s="67"/>
       <c r="DL76" s="67"/>
       <c r="DM76" s="67"/>
       <c r="DN76" s="67"/>
@@ -30376,24 +30248,24 @@
       <c r="DP76" s="67"/>
       <c r="DQ76" s="67"/>
       <c r="DR76" s="67"/>
-      <c r="DS76" s="67" t="s">
-        <v>238</v>
-      </c>
-      <c r="DT76" s="68"/>
-      <c r="DU76" s="68"/>
-      <c r="DV76" s="68"/>
-      <c r="DW76" s="68"/>
-      <c r="DX76" s="68"/>
-      <c r="DY76" s="68"/>
-      <c r="DZ76" s="68"/>
-      <c r="EA76" s="68"/>
-      <c r="EB76" s="68"/>
-      <c r="EC76" s="68"/>
-      <c r="ED76" s="68"/>
-      <c r="EE76" s="68"/>
+      <c r="DS76" s="67"/>
+      <c r="DT76" s="65"/>
+      <c r="DU76" s="65"/>
+      <c r="DV76" s="65"/>
+      <c r="DW76" s="65"/>
+      <c r="DX76" s="65"/>
+      <c r="DY76" s="65"/>
+      <c r="DZ76" s="65"/>
+      <c r="EA76" s="65"/>
+      <c r="EB76" s="65"/>
+      <c r="EC76" s="65"/>
+      <c r="ED76" s="65"/>
+      <c r="EE76" s="65"/>
     </row>
-    <row r="77" customFormat="false" ht="42.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="61"/>
+    <row r="77" customFormat="false" ht="27.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="61" t="s">
+        <v>239</v>
+      </c>
       <c r="B77" s="61"/>
       <c r="C77" s="61"/>
       <c r="D77" s="61"/>
@@ -30402,46 +30274,44 @@
       <c r="G77" s="61"/>
       <c r="H77" s="61"/>
       <c r="I77" s="61"/>
-      <c r="J77" s="67" t="s">
+      <c r="J77" s="61"/>
+      <c r="K77" s="65"/>
+      <c r="L77" s="65"/>
+      <c r="M77" s="65"/>
+      <c r="N77" s="65"/>
+      <c r="O77" s="65"/>
+      <c r="P77" s="65"/>
+      <c r="Q77" s="65"/>
+      <c r="R77" s="65"/>
+      <c r="S77" s="65"/>
+      <c r="T77" s="65"/>
+      <c r="U77" s="65"/>
+      <c r="V77" s="61" t="s">
         <v>239</v>
       </c>
-      <c r="K77" s="68"/>
-      <c r="L77" s="68"/>
-      <c r="M77" s="68"/>
-      <c r="N77" s="68"/>
-      <c r="O77" s="68"/>
-      <c r="P77" s="68"/>
-      <c r="Q77" s="68"/>
-      <c r="R77" s="68"/>
-      <c r="S77" s="68"/>
-      <c r="T77" s="68"/>
-      <c r="U77" s="68"/>
-      <c r="V77" s="67" t="s">
-        <v>239</v>
-      </c>
-      <c r="W77" s="67"/>
-      <c r="X77" s="67"/>
-      <c r="Y77" s="67"/>
-      <c r="Z77" s="67"/>
-      <c r="AA77" s="67"/>
-      <c r="AB77" s="67"/>
-      <c r="AC77" s="67"/>
-      <c r="AD77" s="67"/>
-      <c r="AE77" s="67"/>
-      <c r="AF77" s="69"/>
-      <c r="AG77" s="69"/>
-      <c r="AH77" s="69"/>
-      <c r="AI77" s="69"/>
-      <c r="AJ77" s="69"/>
-      <c r="AK77" s="69"/>
-      <c r="AL77" s="69"/>
-      <c r="AM77" s="69"/>
-      <c r="AN77" s="69"/>
-      <c r="AO77" s="69"/>
-      <c r="AP77" s="69"/>
-      <c r="AQ77" s="69"/>
-      <c r="AR77" s="69"/>
-      <c r="AS77" s="69"/>
+      <c r="W77" s="61"/>
+      <c r="X77" s="61"/>
+      <c r="Y77" s="61"/>
+      <c r="Z77" s="61"/>
+      <c r="AA77" s="61"/>
+      <c r="AB77" s="61"/>
+      <c r="AC77" s="61"/>
+      <c r="AD77" s="61"/>
+      <c r="AE77" s="61"/>
+      <c r="AF77" s="66"/>
+      <c r="AG77" s="66"/>
+      <c r="AH77" s="66"/>
+      <c r="AI77" s="66"/>
+      <c r="AJ77" s="66"/>
+      <c r="AK77" s="66"/>
+      <c r="AL77" s="66"/>
+      <c r="AM77" s="66"/>
+      <c r="AN77" s="66"/>
+      <c r="AO77" s="66"/>
+      <c r="AP77" s="66"/>
+      <c r="AQ77" s="66"/>
+      <c r="AR77" s="66"/>
+      <c r="AS77" s="66"/>
       <c r="AT77" s="67" t="s">
         <v>239</v>
       </c>
@@ -30453,20 +30323,20 @@
       <c r="AZ77" s="67"/>
       <c r="BA77" s="67"/>
       <c r="BB77" s="67"/>
-      <c r="BC77" s="70"/>
-      <c r="BD77" s="70"/>
-      <c r="BE77" s="70"/>
-      <c r="BF77" s="70"/>
-      <c r="BG77" s="70"/>
-      <c r="BH77" s="70"/>
-      <c r="BI77" s="70"/>
-      <c r="BJ77" s="70"/>
-      <c r="BK77" s="70"/>
-      <c r="BL77" s="70"/>
-      <c r="BM77" s="70"/>
-      <c r="BN77" s="70"/>
-      <c r="BO77" s="70"/>
-      <c r="BP77" s="70"/>
+      <c r="BC77" s="66"/>
+      <c r="BD77" s="66"/>
+      <c r="BE77" s="66"/>
+      <c r="BF77" s="66"/>
+      <c r="BG77" s="66"/>
+      <c r="BH77" s="66"/>
+      <c r="BI77" s="66"/>
+      <c r="BJ77" s="66"/>
+      <c r="BK77" s="66"/>
+      <c r="BL77" s="66"/>
+      <c r="BM77" s="66"/>
+      <c r="BN77" s="66"/>
+      <c r="BO77" s="66"/>
+      <c r="BP77" s="66"/>
       <c r="BQ77" s="67" t="s">
         <v>239</v>
       </c>
@@ -30478,20 +30348,20 @@
       <c r="BW77" s="67"/>
       <c r="BX77" s="67"/>
       <c r="BY77" s="67"/>
-      <c r="BZ77" s="68"/>
-      <c r="CA77" s="68"/>
-      <c r="CB77" s="68"/>
-      <c r="CC77" s="68"/>
-      <c r="CD77" s="68"/>
-      <c r="CE77" s="68"/>
-      <c r="CF77" s="68"/>
-      <c r="CG77" s="68"/>
-      <c r="CH77" s="68"/>
-      <c r="CI77" s="68"/>
-      <c r="CJ77" s="68"/>
-      <c r="CK77" s="68"/>
-      <c r="CL77" s="68"/>
-      <c r="CM77" s="68"/>
+      <c r="BZ77" s="65"/>
+      <c r="CA77" s="65"/>
+      <c r="CB77" s="65"/>
+      <c r="CC77" s="65"/>
+      <c r="CD77" s="65"/>
+      <c r="CE77" s="65"/>
+      <c r="CF77" s="65"/>
+      <c r="CG77" s="65"/>
+      <c r="CH77" s="65"/>
+      <c r="CI77" s="65"/>
+      <c r="CJ77" s="65"/>
+      <c r="CK77" s="65"/>
+      <c r="CL77" s="65"/>
+      <c r="CM77" s="65"/>
       <c r="CN77" s="67" t="s">
         <v>239</v>
       </c>
@@ -30503,20 +30373,20 @@
       <c r="CT77" s="67"/>
       <c r="CU77" s="67"/>
       <c r="CV77" s="67"/>
-      <c r="CW77" s="71"/>
-      <c r="CX77" s="71"/>
-      <c r="CY77" s="71"/>
-      <c r="CZ77" s="71"/>
-      <c r="DA77" s="71"/>
-      <c r="DB77" s="71"/>
-      <c r="DC77" s="71"/>
-      <c r="DD77" s="71"/>
-      <c r="DE77" s="71"/>
-      <c r="DF77" s="71"/>
-      <c r="DG77" s="71"/>
-      <c r="DH77" s="71"/>
-      <c r="DI77" s="71"/>
-      <c r="DJ77" s="71"/>
+      <c r="CW77" s="65"/>
+      <c r="CX77" s="65"/>
+      <c r="CY77" s="65"/>
+      <c r="CZ77" s="65"/>
+      <c r="DA77" s="65"/>
+      <c r="DB77" s="65"/>
+      <c r="DC77" s="65"/>
+      <c r="DD77" s="65"/>
+      <c r="DE77" s="65"/>
+      <c r="DF77" s="65"/>
+      <c r="DG77" s="65"/>
+      <c r="DH77" s="65"/>
+      <c r="DI77" s="65"/>
+      <c r="DJ77" s="65"/>
       <c r="DK77" s="67" t="s">
         <v>239</v>
       </c>
@@ -30528,21 +30398,23 @@
       <c r="DQ77" s="67"/>
       <c r="DR77" s="67"/>
       <c r="DS77" s="67"/>
-      <c r="DT77" s="68"/>
-      <c r="DU77" s="68"/>
-      <c r="DV77" s="68"/>
-      <c r="DW77" s="68"/>
-      <c r="DX77" s="68"/>
-      <c r="DY77" s="68"/>
-      <c r="DZ77" s="68"/>
-      <c r="EA77" s="68"/>
-      <c r="EB77" s="68"/>
-      <c r="EC77" s="68"/>
-      <c r="ED77" s="68"/>
-      <c r="EE77" s="68"/>
+      <c r="DT77" s="65"/>
+      <c r="DU77" s="65"/>
+      <c r="DV77" s="65"/>
+      <c r="DW77" s="65"/>
+      <c r="DX77" s="65"/>
+      <c r="DY77" s="65"/>
+      <c r="DZ77" s="65"/>
+      <c r="EA77" s="65"/>
+      <c r="EB77" s="65"/>
+      <c r="EC77" s="65"/>
+      <c r="ED77" s="65"/>
+      <c r="EE77" s="65"/>
     </row>
-    <row r="78" customFormat="false" ht="48.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="61"/>
+    <row r="78" customFormat="false" ht="31.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="61" t="s">
+        <v>240</v>
+      </c>
       <c r="B78" s="61"/>
       <c r="C78" s="61"/>
       <c r="D78" s="61"/>
@@ -30551,46 +30423,44 @@
       <c r="G78" s="61"/>
       <c r="H78" s="61"/>
       <c r="I78" s="61"/>
-      <c r="J78" s="67" t="s">
+      <c r="J78" s="61"/>
+      <c r="K78" s="65"/>
+      <c r="L78" s="65"/>
+      <c r="M78" s="65"/>
+      <c r="N78" s="65"/>
+      <c r="O78" s="65"/>
+      <c r="P78" s="65"/>
+      <c r="Q78" s="65"/>
+      <c r="R78" s="65"/>
+      <c r="S78" s="65"/>
+      <c r="T78" s="65"/>
+      <c r="U78" s="65"/>
+      <c r="V78" s="61" t="s">
         <v>240</v>
       </c>
-      <c r="K78" s="68"/>
-      <c r="L78" s="68"/>
-      <c r="M78" s="68"/>
-      <c r="N78" s="68"/>
-      <c r="O78" s="68"/>
-      <c r="P78" s="68"/>
-      <c r="Q78" s="68"/>
-      <c r="R78" s="68"/>
-      <c r="S78" s="68"/>
-      <c r="T78" s="68"/>
-      <c r="U78" s="68"/>
-      <c r="V78" s="67" t="s">
-        <v>240</v>
-      </c>
-      <c r="W78" s="67"/>
-      <c r="X78" s="67"/>
-      <c r="Y78" s="67"/>
-      <c r="Z78" s="67"/>
-      <c r="AA78" s="67"/>
-      <c r="AB78" s="67"/>
-      <c r="AC78" s="67"/>
-      <c r="AD78" s="67"/>
-      <c r="AE78" s="67"/>
-      <c r="AF78" s="69"/>
-      <c r="AG78" s="69"/>
-      <c r="AH78" s="69"/>
-      <c r="AI78" s="69"/>
-      <c r="AJ78" s="69"/>
-      <c r="AK78" s="69"/>
-      <c r="AL78" s="69"/>
-      <c r="AM78" s="69"/>
-      <c r="AN78" s="69"/>
-      <c r="AO78" s="69"/>
-      <c r="AP78" s="69"/>
-      <c r="AQ78" s="69"/>
-      <c r="AR78" s="69"/>
-      <c r="AS78" s="69"/>
+      <c r="W78" s="61"/>
+      <c r="X78" s="61"/>
+      <c r="Y78" s="61"/>
+      <c r="Z78" s="61"/>
+      <c r="AA78" s="61"/>
+      <c r="AB78" s="61"/>
+      <c r="AC78" s="61"/>
+      <c r="AD78" s="61"/>
+      <c r="AE78" s="61"/>
+      <c r="AF78" s="66"/>
+      <c r="AG78" s="66"/>
+      <c r="AH78" s="66"/>
+      <c r="AI78" s="66"/>
+      <c r="AJ78" s="66"/>
+      <c r="AK78" s="66"/>
+      <c r="AL78" s="66"/>
+      <c r="AM78" s="66"/>
+      <c r="AN78" s="66"/>
+      <c r="AO78" s="66"/>
+      <c r="AP78" s="66"/>
+      <c r="AQ78" s="66"/>
+      <c r="AR78" s="66"/>
+      <c r="AS78" s="66"/>
       <c r="AT78" s="67" t="s">
         <v>240</v>
       </c>
@@ -30602,20 +30472,20 @@
       <c r="AZ78" s="67"/>
       <c r="BA78" s="67"/>
       <c r="BB78" s="67"/>
-      <c r="BC78" s="70"/>
-      <c r="BD78" s="70"/>
-      <c r="BE78" s="70"/>
-      <c r="BF78" s="70"/>
-      <c r="BG78" s="70"/>
-      <c r="BH78" s="70"/>
-      <c r="BI78" s="70"/>
-      <c r="BJ78" s="70"/>
-      <c r="BK78" s="70"/>
-      <c r="BL78" s="70"/>
-      <c r="BM78" s="70"/>
-      <c r="BN78" s="70"/>
-      <c r="BO78" s="70"/>
-      <c r="BP78" s="70"/>
+      <c r="BC78" s="66"/>
+      <c r="BD78" s="66"/>
+      <c r="BE78" s="66"/>
+      <c r="BF78" s="66"/>
+      <c r="BG78" s="66"/>
+      <c r="BH78" s="66"/>
+      <c r="BI78" s="66"/>
+      <c r="BJ78" s="66"/>
+      <c r="BK78" s="66"/>
+      <c r="BL78" s="66"/>
+      <c r="BM78" s="66"/>
+      <c r="BN78" s="66"/>
+      <c r="BO78" s="66"/>
+      <c r="BP78" s="66"/>
       <c r="BQ78" s="67" t="s">
         <v>240</v>
       </c>
@@ -30627,20 +30497,20 @@
       <c r="BW78" s="67"/>
       <c r="BX78" s="67"/>
       <c r="BY78" s="67"/>
-      <c r="BZ78" s="68"/>
-      <c r="CA78" s="68"/>
-      <c r="CB78" s="68"/>
-      <c r="CC78" s="68"/>
-      <c r="CD78" s="68"/>
-      <c r="CE78" s="68"/>
-      <c r="CF78" s="68"/>
-      <c r="CG78" s="68"/>
-      <c r="CH78" s="68"/>
-      <c r="CI78" s="68"/>
-      <c r="CJ78" s="68"/>
-      <c r="CK78" s="68"/>
-      <c r="CL78" s="68"/>
-      <c r="CM78" s="68"/>
+      <c r="BZ78" s="65"/>
+      <c r="CA78" s="65"/>
+      <c r="CB78" s="65"/>
+      <c r="CC78" s="65"/>
+      <c r="CD78" s="65"/>
+      <c r="CE78" s="65"/>
+      <c r="CF78" s="65"/>
+      <c r="CG78" s="65"/>
+      <c r="CH78" s="65"/>
+      <c r="CI78" s="65"/>
+      <c r="CJ78" s="65"/>
+      <c r="CK78" s="65"/>
+      <c r="CL78" s="65"/>
+      <c r="CM78" s="65"/>
       <c r="CN78" s="67" t="s">
         <v>240</v>
       </c>
@@ -30652,20 +30522,20 @@
       <c r="CT78" s="67"/>
       <c r="CU78" s="67"/>
       <c r="CV78" s="67"/>
-      <c r="CW78" s="71"/>
-      <c r="CX78" s="71"/>
-      <c r="CY78" s="71"/>
-      <c r="CZ78" s="71"/>
-      <c r="DA78" s="71"/>
-      <c r="DB78" s="71"/>
-      <c r="DC78" s="71"/>
-      <c r="DD78" s="71"/>
-      <c r="DE78" s="71"/>
-      <c r="DF78" s="71"/>
-      <c r="DG78" s="71"/>
-      <c r="DH78" s="71"/>
-      <c r="DI78" s="71"/>
-      <c r="DJ78" s="71"/>
+      <c r="CW78" s="65"/>
+      <c r="CX78" s="65"/>
+      <c r="CY78" s="65"/>
+      <c r="CZ78" s="65"/>
+      <c r="DA78" s="65"/>
+      <c r="DB78" s="65"/>
+      <c r="DC78" s="65"/>
+      <c r="DD78" s="65"/>
+      <c r="DE78" s="65"/>
+      <c r="DF78" s="65"/>
+      <c r="DG78" s="65"/>
+      <c r="DH78" s="65"/>
+      <c r="DI78" s="65"/>
+      <c r="DJ78" s="65"/>
       <c r="DK78" s="67" t="s">
         <v>240</v>
       </c>
@@ -30677,617 +30547,24 @@
       <c r="DQ78" s="67"/>
       <c r="DR78" s="67"/>
       <c r="DS78" s="67"/>
-      <c r="DT78" s="68"/>
-      <c r="DU78" s="68"/>
-      <c r="DV78" s="68"/>
-      <c r="DW78" s="68"/>
-      <c r="DX78" s="68"/>
-      <c r="DY78" s="68"/>
-      <c r="DZ78" s="68"/>
-      <c r="EA78" s="68"/>
-      <c r="EB78" s="68"/>
-      <c r="EC78" s="68"/>
-      <c r="ED78" s="68"/>
-      <c r="EE78" s="68"/>
+      <c r="DT78" s="65"/>
+      <c r="DU78" s="65"/>
+      <c r="DV78" s="65"/>
+      <c r="DW78" s="65"/>
+      <c r="DX78" s="65"/>
+      <c r="DY78" s="65"/>
+      <c r="DZ78" s="65"/>
+      <c r="EA78" s="65"/>
+      <c r="EB78" s="65"/>
+      <c r="EC78" s="65"/>
+      <c r="ED78" s="65"/>
+      <c r="EE78" s="65"/>
     </row>
-    <row r="79" s="73" customFormat="true" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="72"/>
-      <c r="B79" s="72"/>
-      <c r="J79" s="74"/>
-      <c r="K79" s="70"/>
-      <c r="L79" s="70"/>
-      <c r="M79" s="70"/>
-      <c r="N79" s="70"/>
-      <c r="O79" s="70"/>
-      <c r="P79" s="70"/>
-      <c r="Q79" s="70"/>
-      <c r="R79" s="70"/>
-      <c r="S79" s="70"/>
-      <c r="T79" s="70"/>
-      <c r="U79" s="70"/>
-      <c r="V79" s="72"/>
-      <c r="W79" s="72"/>
-      <c r="AE79" s="74"/>
-      <c r="AF79" s="70"/>
-      <c r="AG79" s="70"/>
-      <c r="AH79" s="70"/>
-      <c r="AI79" s="70"/>
-      <c r="AJ79" s="70"/>
-      <c r="AK79" s="70"/>
-      <c r="AL79" s="70"/>
-      <c r="AM79" s="70"/>
-      <c r="AN79" s="70"/>
-      <c r="AO79" s="70"/>
-      <c r="AP79" s="70"/>
-      <c r="AQ79" s="70"/>
-      <c r="AR79" s="70"/>
-      <c r="AS79" s="70"/>
-      <c r="AT79" s="72"/>
-      <c r="BB79" s="74"/>
-      <c r="BC79" s="70"/>
-      <c r="BD79" s="70"/>
-      <c r="BE79" s="70"/>
-      <c r="BF79" s="70"/>
-      <c r="BG79" s="70"/>
-      <c r="BH79" s="70"/>
-      <c r="BI79" s="70"/>
-      <c r="BJ79" s="70"/>
-      <c r="BK79" s="70"/>
-      <c r="BL79" s="70"/>
-      <c r="BM79" s="70"/>
-      <c r="BN79" s="70"/>
-      <c r="BO79" s="70"/>
-      <c r="BP79" s="70"/>
-      <c r="BQ79" s="72"/>
-      <c r="BY79" s="74"/>
-      <c r="BZ79" s="70"/>
-      <c r="CA79" s="70"/>
-      <c r="CB79" s="70"/>
-      <c r="CC79" s="70"/>
-      <c r="CD79" s="74"/>
-      <c r="CE79" s="70"/>
-      <c r="CF79" s="70"/>
-      <c r="CG79" s="70"/>
-      <c r="CH79" s="70"/>
-      <c r="CI79" s="70"/>
-      <c r="CJ79" s="70"/>
-      <c r="CK79" s="70"/>
-      <c r="CL79" s="70"/>
-      <c r="CM79" s="70"/>
-      <c r="CN79" s="72"/>
-      <c r="CV79" s="74"/>
-      <c r="CW79" s="70"/>
-      <c r="CX79" s="70"/>
-      <c r="CY79" s="70"/>
-      <c r="CZ79" s="70"/>
-      <c r="DA79" s="70"/>
-      <c r="DB79" s="70"/>
-      <c r="DC79" s="70"/>
-      <c r="DD79" s="70"/>
-      <c r="DE79" s="70"/>
-      <c r="DF79" s="70"/>
-      <c r="DG79" s="70"/>
-      <c r="DH79" s="70"/>
-      <c r="DI79" s="70"/>
-      <c r="DJ79" s="70"/>
-      <c r="DK79" s="72"/>
-      <c r="DS79" s="74"/>
-      <c r="DT79" s="70"/>
-      <c r="DU79" s="70"/>
-      <c r="DV79" s="70"/>
-      <c r="DW79" s="70"/>
-      <c r="DX79" s="70"/>
-      <c r="DY79" s="70"/>
-      <c r="DZ79" s="70"/>
-      <c r="EA79" s="70"/>
-      <c r="EB79" s="70"/>
-      <c r="EC79" s="70"/>
-      <c r="ED79" s="70"/>
-      <c r="EE79" s="70"/>
-    </row>
-    <row r="80" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J80" s="74"/>
-      <c r="K80" s="75"/>
-      <c r="L80" s="75"/>
-      <c r="M80" s="75"/>
-      <c r="N80" s="75"/>
-      <c r="O80" s="75"/>
-      <c r="P80" s="75"/>
-      <c r="Q80" s="75"/>
-      <c r="R80" s="75"/>
-      <c r="S80" s="75"/>
-      <c r="T80" s="75"/>
-      <c r="U80" s="75"/>
-      <c r="AE80" s="74"/>
-      <c r="AF80" s="75"/>
-      <c r="AG80" s="75"/>
-      <c r="AH80" s="75"/>
-      <c r="AI80" s="75"/>
-      <c r="AJ80" s="75"/>
-      <c r="AK80" s="75"/>
-      <c r="AL80" s="75"/>
-      <c r="AM80" s="75"/>
-      <c r="AN80" s="75"/>
-      <c r="AO80" s="75"/>
-      <c r="AP80" s="75"/>
-      <c r="AQ80" s="75"/>
-      <c r="AR80" s="75"/>
-      <c r="AS80" s="75"/>
-      <c r="BB80" s="74"/>
-      <c r="BC80" s="75"/>
-      <c r="BD80" s="75"/>
-      <c r="BE80" s="75"/>
-      <c r="BF80" s="75"/>
-      <c r="BG80" s="75"/>
-      <c r="BH80" s="75"/>
-      <c r="BI80" s="75"/>
-      <c r="BJ80" s="75"/>
-      <c r="BK80" s="75"/>
-      <c r="BL80" s="75"/>
-      <c r="BM80" s="75"/>
-      <c r="BN80" s="75"/>
-      <c r="BO80" s="75"/>
-      <c r="BP80" s="75"/>
-      <c r="BY80" s="74"/>
-      <c r="BZ80" s="75"/>
-      <c r="CA80" s="75"/>
-      <c r="CB80" s="75"/>
-      <c r="CC80" s="75"/>
-      <c r="CD80" s="74"/>
-      <c r="CE80" s="75"/>
-      <c r="CF80" s="70"/>
-      <c r="CG80" s="75"/>
-      <c r="CH80" s="75"/>
-      <c r="CI80" s="75"/>
-      <c r="CJ80" s="75"/>
-      <c r="CK80" s="75"/>
-      <c r="CL80" s="75"/>
-      <c r="CM80" s="75"/>
-      <c r="CV80" s="74"/>
-      <c r="CW80" s="75"/>
-      <c r="CX80" s="75"/>
-      <c r="CY80" s="75"/>
-      <c r="CZ80" s="75"/>
-      <c r="DA80" s="75"/>
-      <c r="DB80" s="75"/>
-      <c r="DC80" s="75"/>
-      <c r="DD80" s="75"/>
-      <c r="DE80" s="75"/>
-      <c r="DF80" s="75"/>
-      <c r="DG80" s="75"/>
-      <c r="DH80" s="75"/>
-      <c r="DI80" s="75"/>
-      <c r="DJ80" s="75"/>
-      <c r="DS80" s="74"/>
-      <c r="DT80" s="75"/>
-      <c r="DU80" s="75"/>
-      <c r="DV80" s="75"/>
-      <c r="DW80" s="75"/>
-      <c r="DX80" s="75"/>
-      <c r="DY80" s="75"/>
-      <c r="DZ80" s="75"/>
-      <c r="EA80" s="75"/>
-      <c r="EB80" s="75"/>
-      <c r="EC80" s="75"/>
-      <c r="ED80" s="70"/>
-      <c r="EE80" s="75"/>
-    </row>
-    <row r="81" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K81" s="75"/>
-      <c r="L81" s="75"/>
-      <c r="M81" s="75"/>
-      <c r="N81" s="75"/>
-      <c r="O81" s="75"/>
-      <c r="P81" s="75"/>
-      <c r="Q81" s="75"/>
-      <c r="R81" s="75"/>
-      <c r="S81" s="75"/>
-      <c r="T81" s="75"/>
-      <c r="U81" s="75"/>
-      <c r="AF81" s="75"/>
-      <c r="AG81" s="75"/>
-      <c r="AH81" s="75"/>
-      <c r="AI81" s="75"/>
-      <c r="AJ81" s="75"/>
-      <c r="AK81" s="75"/>
-      <c r="AL81" s="75"/>
-      <c r="AM81" s="75"/>
-      <c r="AN81" s="75"/>
-      <c r="AO81" s="75"/>
-      <c r="AP81" s="75"/>
-      <c r="AQ81" s="75"/>
-      <c r="AR81" s="75"/>
-      <c r="AS81" s="75"/>
-      <c r="BC81" s="75"/>
-      <c r="BD81" s="75"/>
-      <c r="BE81" s="75"/>
-      <c r="BF81" s="75"/>
-      <c r="BG81" s="75"/>
-      <c r="BH81" s="75"/>
-      <c r="BI81" s="75"/>
-      <c r="BJ81" s="75"/>
-      <c r="BK81" s="75"/>
-      <c r="BL81" s="75"/>
-      <c r="BM81" s="75"/>
-      <c r="BN81" s="75"/>
-      <c r="BO81" s="75"/>
-      <c r="BP81" s="75"/>
-      <c r="BZ81" s="75"/>
-      <c r="CA81" s="75"/>
-      <c r="CB81" s="75"/>
-      <c r="CC81" s="75"/>
-      <c r="CE81" s="75"/>
-      <c r="CF81" s="70"/>
-      <c r="CG81" s="75"/>
-      <c r="CH81" s="75"/>
-      <c r="CI81" s="75"/>
-      <c r="CJ81" s="75"/>
-      <c r="CK81" s="75"/>
-      <c r="CL81" s="75"/>
-      <c r="CM81" s="75"/>
-      <c r="CW81" s="75"/>
-      <c r="CX81" s="75"/>
-      <c r="CY81" s="75"/>
-      <c r="CZ81" s="75"/>
-      <c r="DA81" s="75"/>
-      <c r="DB81" s="76" t="s">
-        <v>241</v>
-      </c>
-      <c r="DC81" s="77"/>
-      <c r="DD81" s="75"/>
-      <c r="DE81" s="75"/>
-      <c r="DF81" s="75"/>
-      <c r="DG81" s="75"/>
-      <c r="DH81" s="75"/>
-      <c r="DI81" s="75"/>
-      <c r="DJ81" s="75"/>
-      <c r="DT81" s="75"/>
-      <c r="DU81" s="75"/>
-      <c r="DV81" s="75"/>
-      <c r="DW81" s="75"/>
-      <c r="DX81" s="75"/>
-      <c r="DY81" s="75"/>
-      <c r="DZ81" s="75"/>
-      <c r="EA81" s="75"/>
-      <c r="EB81" s="75"/>
-      <c r="EC81" s="75"/>
-      <c r="ED81" s="70"/>
-      <c r="EE81" s="75"/>
-    </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L82" s="77"/>
-      <c r="T82" s="77"/>
-      <c r="AS82" s="77"/>
-      <c r="DB82" s="78" t="s">
-        <v>242</v>
-      </c>
-      <c r="DC82" s="77"/>
-    </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L83" s="77"/>
-      <c r="T83" s="77"/>
-      <c r="AS83" s="77"/>
-      <c r="DB83" s="78" t="s">
-        <v>243</v>
-      </c>
-      <c r="DC83" s="77"/>
-    </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L84" s="77"/>
-      <c r="T84" s="77"/>
-      <c r="AS84" s="77"/>
-      <c r="DB84" s="79" t="s">
-        <v>242</v>
-      </c>
-      <c r="DC84" s="77"/>
-    </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L85" s="77"/>
-      <c r="T85" s="77"/>
-      <c r="AS85" s="77"/>
-    </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L86" s="77"/>
-      <c r="T86" s="77"/>
-      <c r="AS86" s="77"/>
-    </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L87" s="77"/>
-      <c r="T87" s="77"/>
-      <c r="AS87" s="77"/>
-      <c r="DB87" s="76" t="s">
-        <v>244</v>
-      </c>
-      <c r="DC87" s="77"/>
-    </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L88" s="77"/>
-      <c r="T88" s="77"/>
-      <c r="AS88" s="77"/>
-      <c r="DB88" s="78" t="s">
-        <v>245</v>
-      </c>
-      <c r="DC88" s="77"/>
-    </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L89" s="77"/>
-      <c r="T89" s="77"/>
-      <c r="AS89" s="77"/>
-      <c r="DB89" s="79" t="s">
-        <v>246</v>
-      </c>
-      <c r="DC89" s="77"/>
-    </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L90" s="77"/>
-      <c r="T90" s="77"/>
-      <c r="AS90" s="77"/>
-    </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L91" s="77"/>
-      <c r="T91" s="77"/>
-      <c r="AS91" s="77"/>
-    </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L92" s="77"/>
-      <c r="T92" s="77"/>
-      <c r="AS92" s="77"/>
-      <c r="DB92" s="76" t="s">
-        <v>247</v>
-      </c>
-      <c r="DC92" s="77"/>
-    </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L93" s="77"/>
-      <c r="T93" s="77"/>
-      <c r="AS93" s="77"/>
-      <c r="DB93" s="78" t="s">
-        <v>248</v>
-      </c>
-      <c r="DC93" s="77"/>
-    </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L94" s="77"/>
-      <c r="T94" s="77"/>
-      <c r="AS94" s="77"/>
-      <c r="DB94" s="78" t="s">
-        <v>249</v>
-      </c>
-      <c r="DC94" s="77"/>
-    </row>
-    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L95" s="77"/>
-      <c r="T95" s="77"/>
-      <c r="AS95" s="77"/>
-      <c r="DB95" s="79" t="s">
-        <v>250</v>
-      </c>
-      <c r="DC95" s="77"/>
-    </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L96" s="77"/>
-      <c r="T96" s="77"/>
-      <c r="AS96" s="77"/>
-    </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L97" s="77"/>
-      <c r="T97" s="77"/>
-      <c r="AS97" s="77"/>
-    </row>
-    <row r="98" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K98" s="3"/>
-      <c r="L98" s="77"/>
-      <c r="M98" s="3"/>
-      <c r="N98" s="3"/>
-      <c r="O98" s="3"/>
-      <c r="P98" s="3"/>
-      <c r="Q98" s="3"/>
-      <c r="R98" s="3"/>
-      <c r="S98" s="3"/>
-      <c r="T98" s="77"/>
-      <c r="U98" s="3"/>
-      <c r="AF98" s="3"/>
-      <c r="AG98" s="3"/>
-      <c r="AH98" s="3"/>
-      <c r="AI98" s="3"/>
-      <c r="AJ98" s="3"/>
-      <c r="AK98" s="3"/>
-      <c r="AR98" s="3"/>
-      <c r="AS98" s="77"/>
-      <c r="BC98" s="3"/>
-      <c r="BD98" s="3"/>
-      <c r="BE98" s="3"/>
-      <c r="BF98" s="3"/>
-      <c r="BG98" s="3"/>
-      <c r="BH98" s="3"/>
-      <c r="BO98" s="3"/>
-      <c r="DB98" s="2" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="99" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K99" s="3"/>
-      <c r="L99" s="77"/>
-      <c r="M99" s="3"/>
-      <c r="N99" s="3"/>
-      <c r="O99" s="3"/>
-      <c r="P99" s="3"/>
-      <c r="Q99" s="3"/>
-      <c r="R99" s="3"/>
-      <c r="S99" s="3"/>
-      <c r="T99" s="77"/>
-      <c r="U99" s="3"/>
-      <c r="AF99" s="3"/>
-      <c r="AG99" s="3"/>
-      <c r="AH99" s="3"/>
-      <c r="AI99" s="3"/>
-      <c r="AJ99" s="3"/>
-      <c r="AK99" s="3"/>
-      <c r="AR99" s="3"/>
-      <c r="AS99" s="77"/>
-      <c r="BC99" s="3"/>
-      <c r="BD99" s="3"/>
-      <c r="BE99" s="3"/>
-      <c r="BF99" s="3"/>
-      <c r="BG99" s="3"/>
-      <c r="BH99" s="3"/>
-      <c r="BO99" s="3"/>
-      <c r="DB99" s="77" t="s">
-        <v>251</v>
-      </c>
-      <c r="DC99" s="77"/>
-    </row>
-    <row r="100" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K100" s="3"/>
-      <c r="L100" s="77"/>
-      <c r="M100" s="3"/>
-      <c r="N100" s="3"/>
-      <c r="O100" s="3"/>
-      <c r="P100" s="3"/>
-      <c r="Q100" s="3"/>
-      <c r="R100" s="3"/>
-      <c r="S100" s="3"/>
-      <c r="T100" s="77"/>
-      <c r="U100" s="3"/>
-      <c r="AF100" s="3"/>
-      <c r="AG100" s="3"/>
-      <c r="AH100" s="3"/>
-      <c r="AI100" s="3"/>
-      <c r="AJ100" s="3"/>
-      <c r="AK100" s="3"/>
-      <c r="AR100" s="3"/>
-      <c r="AS100" s="77"/>
-      <c r="BC100" s="3"/>
-      <c r="BD100" s="3"/>
-      <c r="BE100" s="3"/>
-      <c r="BF100" s="3"/>
-      <c r="BG100" s="3"/>
-      <c r="BH100" s="3"/>
-      <c r="BO100" s="3"/>
-    </row>
-    <row r="101" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K101" s="3"/>
-      <c r="L101" s="77"/>
-      <c r="M101" s="3"/>
-      <c r="N101" s="3"/>
-      <c r="O101" s="3"/>
-      <c r="P101" s="3"/>
-      <c r="Q101" s="3"/>
-      <c r="R101" s="3"/>
-      <c r="S101" s="3"/>
-      <c r="T101" s="77"/>
-      <c r="U101" s="3"/>
-      <c r="AF101" s="3"/>
-      <c r="AG101" s="3"/>
-      <c r="AH101" s="3"/>
-      <c r="AI101" s="3"/>
-      <c r="AJ101" s="3"/>
-      <c r="AK101" s="3"/>
-      <c r="AR101" s="3"/>
-      <c r="AS101" s="77"/>
-      <c r="BC101" s="3"/>
-      <c r="BD101" s="3"/>
-      <c r="BE101" s="3"/>
-      <c r="BF101" s="3"/>
-      <c r="BG101" s="3"/>
-      <c r="BH101" s="3"/>
-      <c r="BO101" s="3"/>
-    </row>
-    <row r="102" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K102" s="3"/>
-      <c r="L102" s="77"/>
-      <c r="M102" s="3"/>
-      <c r="N102" s="3"/>
-      <c r="O102" s="3"/>
-      <c r="P102" s="3"/>
-      <c r="Q102" s="3"/>
-      <c r="R102" s="3"/>
-      <c r="S102" s="3"/>
-      <c r="T102" s="77"/>
-      <c r="U102" s="3"/>
-      <c r="AF102" s="3"/>
-      <c r="AG102" s="3"/>
-      <c r="AH102" s="3"/>
-      <c r="AI102" s="3"/>
-      <c r="AJ102" s="3"/>
-      <c r="AK102" s="3"/>
-      <c r="AR102" s="3"/>
-      <c r="AS102" s="77"/>
-      <c r="BC102" s="3"/>
-      <c r="BD102" s="3"/>
-      <c r="BE102" s="3"/>
-      <c r="BF102" s="3"/>
-      <c r="BG102" s="3"/>
-      <c r="BH102" s="3"/>
-      <c r="BO102" s="3"/>
-      <c r="DB102" s="2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="103" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K103" s="3"/>
-      <c r="L103" s="77"/>
-      <c r="M103" s="3"/>
-      <c r="N103" s="3"/>
-      <c r="O103" s="3"/>
-      <c r="P103" s="3"/>
-      <c r="Q103" s="3"/>
-      <c r="R103" s="3"/>
-      <c r="S103" s="3"/>
-      <c r="T103" s="77"/>
-      <c r="U103" s="3"/>
-      <c r="AF103" s="3"/>
-      <c r="AG103" s="3"/>
-      <c r="AH103" s="3"/>
-      <c r="AI103" s="3"/>
-      <c r="AJ103" s="3"/>
-      <c r="AK103" s="3"/>
-      <c r="AR103" s="3"/>
-      <c r="AS103" s="77"/>
-      <c r="BC103" s="3"/>
-      <c r="BD103" s="3"/>
-      <c r="BE103" s="3"/>
-      <c r="BF103" s="3"/>
-      <c r="BG103" s="3"/>
-      <c r="BH103" s="3"/>
-      <c r="BO103" s="3"/>
-      <c r="DB103" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="104" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K104" s="3"/>
-      <c r="L104" s="3"/>
-      <c r="M104" s="3"/>
-      <c r="N104" s="3"/>
-      <c r="O104" s="3"/>
-      <c r="P104" s="3"/>
-      <c r="Q104" s="3"/>
-      <c r="R104" s="3"/>
-      <c r="S104" s="3"/>
-      <c r="T104" s="3"/>
-      <c r="U104" s="3"/>
-      <c r="AF104" s="3"/>
-      <c r="AG104" s="3"/>
-      <c r="AH104" s="3"/>
-      <c r="AI104" s="3"/>
-      <c r="AJ104" s="3"/>
-      <c r="AK104" s="3"/>
-      <c r="AR104" s="3"/>
-      <c r="AS104" s="3"/>
-      <c r="BC104" s="3"/>
-      <c r="BD104" s="3"/>
-      <c r="BE104" s="3"/>
-      <c r="BF104" s="3"/>
-      <c r="BG104" s="3"/>
-      <c r="BH104" s="3"/>
-      <c r="BO104" s="3"/>
-      <c r="DB104" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
+    <row r="79" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="80" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="439">
+  <mergeCells count="477">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="F1:J1"/>
     <mergeCell ref="K1:U1"/>
@@ -31711,24 +30988,62 @@
     <mergeCell ref="BR69:BY69"/>
     <mergeCell ref="CO69:CV69"/>
     <mergeCell ref="DL69:DS69"/>
-    <mergeCell ref="A70:I78"/>
+    <mergeCell ref="A70:J70"/>
+    <mergeCell ref="V70:AE70"/>
+    <mergeCell ref="AT70:BB70"/>
+    <mergeCell ref="BQ70:BY70"/>
+    <mergeCell ref="CN70:CV70"/>
+    <mergeCell ref="DK70:DS70"/>
+    <mergeCell ref="A71:J71"/>
+    <mergeCell ref="V71:AE71"/>
+    <mergeCell ref="AT71:BB71"/>
+    <mergeCell ref="BQ71:BY71"/>
+    <mergeCell ref="CN71:CV71"/>
+    <mergeCell ref="DK71:DS71"/>
+    <mergeCell ref="A72:J72"/>
+    <mergeCell ref="V72:AE72"/>
+    <mergeCell ref="AT72:BB72"/>
+    <mergeCell ref="BQ72:BY72"/>
+    <mergeCell ref="CN72:CV72"/>
+    <mergeCell ref="DK72:DS72"/>
+    <mergeCell ref="A73:J73"/>
     <mergeCell ref="V73:AE73"/>
     <mergeCell ref="AT73:BB73"/>
     <mergeCell ref="BQ73:BY73"/>
     <mergeCell ref="CN73:CV73"/>
     <mergeCell ref="DK73:DS73"/>
+    <mergeCell ref="A74:J74"/>
+    <mergeCell ref="V74:AE74"/>
+    <mergeCell ref="AT74:BB74"/>
+    <mergeCell ref="BQ74:BY74"/>
+    <mergeCell ref="CN74:CV74"/>
+    <mergeCell ref="DK74:DS74"/>
+    <mergeCell ref="A75:J75"/>
+    <mergeCell ref="V75:AE75"/>
+    <mergeCell ref="AT75:BB75"/>
+    <mergeCell ref="BQ75:BY75"/>
+    <mergeCell ref="CN75:CV75"/>
+    <mergeCell ref="DK75:DS75"/>
+    <mergeCell ref="A76:J76"/>
+    <mergeCell ref="V76:AE76"/>
+    <mergeCell ref="AT76:BB76"/>
+    <mergeCell ref="BQ76:BY76"/>
+    <mergeCell ref="CN76:CV76"/>
+    <mergeCell ref="DK76:DS76"/>
+    <mergeCell ref="A77:J77"/>
     <mergeCell ref="V77:AE77"/>
     <mergeCell ref="AT77:BB77"/>
     <mergeCell ref="BQ77:BY77"/>
     <mergeCell ref="CN77:CV77"/>
     <mergeCell ref="DK77:DS77"/>
+    <mergeCell ref="A78:J78"/>
     <mergeCell ref="V78:AE78"/>
     <mergeCell ref="AT78:BB78"/>
     <mergeCell ref="BQ78:BY78"/>
     <mergeCell ref="CN78:CV78"/>
     <mergeCell ref="DK78:DS78"/>
   </mergeCells>
-  <conditionalFormatting sqref="BC44:BC47 AJ31 BK31 BK43:BL43 BK48:BL48 BK55:BL55 DE43:DF43 DE55:DF55 DE48:DF48 DE24:DF31 CL24:CL30 CL70:CM70 DD70:DJ70 AS31 BC31:BD31 AH31 BC43:BD43 BC48:BD48 AG48:AH48 BC55:BD55 AG55:AH55 BF43 AL43 BF55 AL55 BF48 AL48 BC70:BP70 AF70:AO70 AS70 BZ70:CC70 CW70:CZ70 AF43:AH43 AS48 AS43 CK24">
+  <conditionalFormatting sqref="BC44:BC47 AJ31 BK31 BK43:BL43 BK48:BL48 BK55:BL55 DE43:DF43 DE55:DF55 DE48:DF48 DE24:DF31 CL24:CL30 CL70:CM70 DD70:DJ70 AS31 BC31:BD31 AH31 BC43:BD43 BC48:BD48 AG48:AH48 BC55:BD55 AG55:AH55 BF43 AL43 BF55 AL55 BF48 AL48 BD70:BP70 AF70:AO70 AS70 BZ70:CC70 CW70:CZ70 AF43:AH43 AS48 AS43 CK24">
     <cfRule type="cellIs" priority="2" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
       <formula>0</formula>
@@ -31740,13 +31055,13 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ19 AJ23 AJ31 AJ37:AJ42 AJ46:AJ48 AJ55 AJ13:AJ14 BK31 BK23 BK19 CC13 BK13:BL13 BK43:BL43 BK48:BL48 BK55:BL55 DE13:DF13 CL13:CM13 DE43:DF43 DE48:DF48 DE55:DF55 CL20:CL22 DE19:DF31 CL24:CL30 CL70:CM70 DD70:DJ70 AS13 BC43:BD43 BC48:BD48 AG48:AH48 BC55:BD55 AG55:AH55 BC13:BD13 AG13:AH13 BC19:BD19 BC15:BC18 BC23:BD23 BC20:BC22 BC31:BD31 BC24:BC30 AH15:AH31 BF13 AL13 BF43 AL43 BF48 AL48 BF55 AL55 BC70:BP70 AS19 AS70 AF70:AO70 BZ70:CC70 CW70:CZ70 AF43:AH43 AS48 AS43 AS31 AS23 CK24">
+  <conditionalFormatting sqref="AJ19 AJ23 AJ31 AJ37:AJ42 AJ46:AJ48 AJ55 AJ13:AJ14 BK31 BK23 BK19 CC13 BK13:BL13 BK43:BL43 BK48:BL48 BK55:BL55 DE13:DF13 CL13:CM13 DE43:DF43 DE48:DF48 DE55:DF55 CL20:CL22 DE19:DF31 CL24:CL30 CL70:CM70 DD70:DJ70 AS13 BC43:BD43 BC48:BD48 AG48:AH48 BC55:BD55 AG55:AH55 BC13:BD13 AG13:AH13 BC19:BD19 BC15:BC18 BC23:BD23 BC20:BC22 BC31:BD31 BC24:BC30 AH15:AH31 BF13 AL13 BF43 AL43 BF48 AL48 BF55 AL55 BD70:BP70 AS19 AS70 AF70:AO70 BZ70:CC70 CW70:CZ70 AF43:AH43 AS48 AS43 AS31 AS23 CK24">
     <cfRule type="cellIs" priority="4" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>0</formula>
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ19 AJ23 AJ31 AJ37:AJ42 AJ46:AJ48 AJ55 AJ13:AJ14 BK31 BK23 BK19 CC13 BK13:BL13 BK43:BL43 BK48:BL48 BK55:BL55 DE13:DF13 CL13:CM13 DE43:DF43 DE48:DF48 DE55:DF55 CL20:CL22 DE19:DF31 CL24:CL30 CL70:CM70 DD70:DJ70 AS13 BC43:BD43 BC48:BD48 AG48:AH48 BC55:BD55 AG55:AH55 BC13:BD13 AG13:AH13 BC19:BD19 BC15:BC18 BC23:BD23 BC20:BC22 BC31:BD31 BC24:BC30 AH15:AH31 BF13 AL13 BF43 AL43 BF48 AL48 BF55 AL55 BC70:BP70 AS19 AS70 AF70:AO70 BZ70:CC70 CW70:CZ70 AF43:AH43 AS48 AS43 AS31 AS23 CK24">
+  <conditionalFormatting sqref="AJ19 AJ23 AJ31 AJ37:AJ42 AJ46:AJ48 AJ55 AJ13:AJ14 BK31 BK23 BK19 CC13 BK13:BL13 BK43:BL43 BK48:BL48 BK55:BL55 DE13:DF13 CL13:CM13 DE43:DF43 DE48:DF48 DE55:DF55 CL20:CL22 DE19:DF31 CL24:CL30 CL70:CM70 DD70:DJ70 AS13 BC43:BD43 BC48:BD48 AG48:AH48 BC55:BD55 AG55:AH55 BC13:BD13 AG13:AH13 BC19:BD19 BC15:BC18 BC23:BD23 BC20:BC22 BC31:BD31 BC24:BC30 AH15:AH31 BF13 AL13 BF43 AL43 BF48 AL48 BF55 AL55 BD70:BP70 AS19 AS70 AF70:AO70 BZ70:CC70 CW70:CZ70 AF43:AH43 AS48 AS43 AS31 AS23 CK24">
     <cfRule type="cellIs" priority="5" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>1</formula>
     </cfRule>
@@ -31754,13 +31069,13 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CL70:CM70 DD70:DJ70 AS70 BC70:BP70 AF70:AO70 BZ70:CC70 CW70:CZ70">
+  <conditionalFormatting sqref="CL70:CM70 DD70:DJ70 AS70 BD70:BP70 AF70:AO70 BZ70:CC70 CW70:CZ70">
     <cfRule type="cellIs" priority="7" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>0</formula>
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CL70:CM70 DD70:DJ70 AS70 BC70:BP70 AF70:AO70 BZ70:CC70 CW70:CZ70">
+  <conditionalFormatting sqref="CL70:CM70 DD70:DJ70 AS70 BD70:BP70 AF70:AO70 BZ70:CC70 CW70:CZ70">
     <cfRule type="cellIs" priority="8" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>1</formula>
     </cfRule>
@@ -51905,6 +51220,40 @@
       <formula>1</formula>
     </cfRule>
     <cfRule type="cellIs" priority="4027" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="297">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BC70">
+    <cfRule type="cellIs" priority="4028" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BC70">
+    <cfRule type="cellIs" priority="4029" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>0</formula>
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BC70">
+    <cfRule type="cellIs" priority="4030" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4031" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BC70">
+    <cfRule type="cellIs" priority="4032" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>0</formula>
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BC70">
+    <cfRule type="cellIs" priority="4033" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4034" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>